<commit_message>
Added No of Tokens
</commit_message>
<xml_diff>
--- a/alpha/token_generated.xlsx
+++ b/alpha/token_generated.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T911"/>
+  <dimension ref="A1:T917"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,13 +565,13 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>1675054925</v>
+        <v>1675484310</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>681740</v>
+        <v>681746</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -588,7 +588,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>{'rate': 1.5023072198464174, 'diff': 0.74, 'diff7d': 7.17, 'ts': 1675055760, 'marketCapUsd': 210691674.33389905, 'availableSupply': 140245398.24513277, 'volume24h': 22726988.47429863, 'volDiff1': 5.388808019754208, 'volDiff7': 22.67959855946873, 'volDiff30': 23.92982817234494, 'diff30d': 46.30755657809274, 'bid': 4.01, 'currency': 'USD'}</t>
+          <t>{'rate': 1.5410176412870102, 'diff': 2.05, 'diff7d': 0.88, 'ts': 1675485960, 'marketCapUsd': 216120632.80507192, 'availableSupply': 140245398.24513277, 'volume24h': 43191361.13143887, 'volDiff1': 53.835135669748354, 'volDiff7': -0.2637450944619246, 'volDiff30': 46.62904389082303, 'diff30d': 43.696005590618626, 'bid': 4.01, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O2" t="n">
@@ -844,7 +844,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>28677949262528039556210596</t>
+          <t>28669391215640011051701865</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -853,13 +853,13 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>1675037055</v>
+        <v>1675480877</v>
       </c>
       <c r="I6" t="n">
-        <v>16303</v>
+        <v>16319</v>
       </c>
       <c r="J6" t="n">
-        <v>85431</v>
+        <v>85422</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
@@ -876,7 +876,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>{'rate': 0.85, 'diff': 5.84, 'diff7d': 2.32, 'ts': 1675055460, 'marketCapUsd': 21091270.311484482, 'availableSupply': 0, 'volume24h': 262252.3728356, 'volDiff1': 6824.207509867162, 'volDiff7': 325.7441892998955, 'volDiff30': 353.6155613737784, 'bid': 5.5, 'diff30d': 46.5051870703077, 'currency': 'USD'}</t>
+          <t>{'rate': 0.8543000000000001, 'diff': 3.26, 'diff7d': 2.46, 'ts': 1675482600, 'marketCapUsd': 21552820.197361533, 'availableSupply': 0, 'volume24h': 263181.51887405023, 'volDiff1': 3952.2193906470634, 'volDiff7': 286.15741964096475, 'volDiff30': 809.9010799111021, 'bid': 5.5, 'diff30d': 46.5051870703077, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O6" t="n">
@@ -935,13 +935,13 @@
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
-        <v>1675001349</v>
+        <v>1675476441</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>5339</v>
+        <v>5335</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
@@ -1152,7 +1152,7 @@
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
-        <v>1673894203</v>
+        <v>1675202990</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>{'rate': 0.0003355758105987665, 'diff': 2.32, 'diff7d': 3.11, 'ts': 1675054200, 'marketCapUsd': 59767.15624763299, 'availableSupply': 178103291, 'volume24h': 0, 'volDiff7': -100, 'volDiff30': -91.52410575427685, 'volDiff1': -100, 'bid': 0.00031574, 'currency': 'USD'}</t>
+          <t>{'rate': 0.0003328728664401671, 'diff': -0.28, 'diff7d': 1.74, 'ts': 1675482600, 'marketCapUsd': 59285.75299759722, 'availableSupply': 178103291, 'volume24h': 0, 'volDiff7': 8026.704440279069, 'volDiff30': -88.09588207451486, 'volDiff1': -100, 'bid': 0.00031574, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O10" t="n">
@@ -1306,7 +1306,7 @@
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="n">
-        <v>1674983648</v>
+        <v>1675082595</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
@@ -1387,7 +1387,7 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>1666204734</v>
+        <v>1675325662</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
@@ -1478,7 +1478,7 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>{'rate': 3.277304189848241e-05, 'diff': 2.66, 'diff7d': 0.27, 'ts': 1675054200, 'marketCapUsd': 4915.891338107501, 'availableSupply': 149998018.29, 'volume24h': 0, 'volDiff7': -100, 'volDiff30': -100, 'bid': 6.013e-05, 'volDiff1': -100, 'currency': 'USD'}</t>
+          <t>{'rate': 3.309394602221032e-05, 'diff': 0.82, 'diff7d': 3.49, 'ts': 1675482600, 'marketCapUsd': 4964.026320727776, 'availableSupply': 149998018.29, 'volume24h': 0, 'volDiff7': -100, 'volDiff30': -100, 'bid': 6.013e-05, 'volDiff1': -100, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O14" t="n">
@@ -1532,7 +1532,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>139582563327718487681327678</t>
+          <t>137383746698825282996231233</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1541,13 +1541,13 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>1674971416</v>
+        <v>1675464656</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>443891</v>
+        <v>443880</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
@@ -2833,13 +2833,13 @@
         </is>
       </c>
       <c r="H34" t="n">
-        <v>1674992324</v>
+        <v>1675479270</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>235918</v>
+        <v>235922</v>
       </c>
       <c r="K34" t="inlineStr">
         <is>
@@ -2856,7 +2856,7 @@
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>{'rate': 6.180311781739225e-05, 'diff': 3.35, 'diff7d': 7, 'ts': 1675055460, 'marketCapUsd': 494424.942539138, 'availableSupply': 8000000000, 'volume24h': 20820.103920966052, 'volDiff1': 11.178206332692014, 'volDiff7': 6.847877316923601, 'volDiff30': -45.84126603579216, 'diff30d': -58.39820215103342, 'bid': 0.00024405, 'currency': 'USD'}</t>
+          <t>{'rate': 6.487579099250692e-05, 'diff': 4.04, 'diff7d': 8.76, 'ts': 1675485660, 'marketCapUsd': 519006.32794005534, 'availableSupply': 8000000000, 'volume24h': 22200.949721466917, 'volDiff1': 14.986253022296921, 'volDiff7': 15.16749230617198, 'volDiff30': -36.86650993695723, 'diff30d': -58.39820215103342, 'bid': 0.00024405, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O34" t="n">
@@ -3319,7 +3319,7 @@
         </is>
       </c>
       <c r="H41" t="n">
-        <v>1675053525</v>
+        <v>1675351918</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
@@ -3399,7 +3399,7 @@
         </is>
       </c>
       <c r="H42" t="n">
-        <v>1675055536</v>
+        <v>1675484703</v>
       </c>
       <c r="I42" t="n">
         <v>21598</v>
@@ -3422,7 +3422,7 @@
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>{'rate': 7.494744394781959, 'diff': 1.78, 'diff7d': 13.02, 'ts': 1675055760, 'marketCapUsd': 203564344.56378514, 'availableSupply': 27160945.56947293, 'volume24h': 5658662.15949956, 'volDiff1': -2.840637361668186, 'volDiff7': 130.17758835193035, 'volDiff30': 100.4804083274021, 'diff30d': 66.50259020229922, 'bid': 24.01, 'currency': 'USD'}</t>
+          <t>{'rate': 8.411374050048257, 'diff': 10.37, 'diff7d': 8.69, 'ts': 1675485960, 'marketCapUsd': 228737941.7727341, 'availableSupply': 27193885.37612613, 'volume24h': 24635819.47417355, 'volDiff1': 121.46041874310575, 'volDiff7': -37.955743436364465, 'volDiff30': 129.88786512307584, 'diff30d': 81.8229266637351, 'bid': 24.01, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O42" t="n">
@@ -3741,13 +3741,13 @@
         </is>
       </c>
       <c r="H47" t="n">
-        <v>1675039733</v>
+        <v>1675422648</v>
       </c>
       <c r="I47" t="n">
         <v>1</v>
       </c>
       <c r="J47" t="n">
-        <v>127349</v>
+        <v>127348</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
@@ -3764,7 +3764,7 @@
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>{'rate': 0.0007356775032345585, 'diff': -1.33, 'diff7d': -5.2, 'ts': 1675055460, 'marketCapUsd': 389608.7574153686, 'availableSupply': 529591778.6018642, 'volume24h': 13480.41308734838, 'volDiff1': -10.019222524374754, 'volDiff7': 15.529181817048453, 'volDiff30': 7.277216097318842, 'bid': 0.00113056, 'currency': 'USD'}</t>
+          <t>{'rate': 0.000826087097398639, 'diff': 7.56, 'diff7d': 11.41, 'ts': 1675485660, 'marketCapUsd': 437488.9351913967, 'availableSupply': 529591778.6018642, 'volume24h': 16997.719225915298, 'volDiff1': 13.58171346915941, 'volDiff7': -5.5348302071814, 'volDiff30': 12.913769014501767, 'bid': 0.00113056, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O47" t="n">
@@ -4014,18 +4014,18 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>3943372046804458044127084</t>
+          <t>3923494324011103994061606</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="n">
-        <v>1675055228</v>
+        <v>1675485883</v>
       </c>
       <c r="I51" t="n">
-        <v>68521120</v>
+        <v>68592878</v>
       </c>
       <c r="J51" t="n">
-        <v>702797</v>
+        <v>706016</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
@@ -4042,7 +4042,7 @@
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>{'rate': 1633.5885623103566, 'diff': 2.41, 'diff7d': -0.12, 'ts': 1675055760, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 931149510.4015378, 'volDiff1': 12.377054982062546, 'volDiff7': 6.7032981582078435, 'volDiff30': 82.50745591628018, 'diff30d': 36.35963756872093, 'bid': 2872.01, 'currency': 'USD'}</t>
+          <t>{'rate': 1652.8946716895518, 'diff': 0.57, 'diff7d': 3.22, 'ts': 1675485960, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 1338823650.039306, 'volDiff1': -22.03788853060105, 'volDiff7': 13.222404524238641, 'volDiff30': 125.9812756168599, 'diff30d': 32.080277048668194, 'bid': 2872.01, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O51" t="n">
@@ -5110,7 +5110,7 @@
       </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>{'rate': 0.0033215935886464704, 'diff': 78.81, 'diff7d': -39.14, 'ts': 1675054200, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 11290.215463652754, 'volDiff1': 114826.76188700652, 'volDiff7': -8.617163636363529, 'volDiff30': -62.59859075184774, 'bid': 0.06556, 'currency': 'USD'}</t>
+          <t>{'rate': 0.0035038654256030425, 'diff': -42.74, 'diff7d': -41.73, 'ts': 1675482600, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 9900.917325126127, 'volDiff1': -99.61617395953613, 'volDiff7': 57.29510302576364, 'volDiff30': -56.35349565813623, 'bid': 0.06556, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O66" t="n">
@@ -5165,13 +5165,13 @@
         </is>
       </c>
       <c r="H67" t="n">
-        <v>1674977657</v>
+        <v>1675396800</v>
       </c>
       <c r="I67" t="n">
         <v>0</v>
       </c>
       <c r="J67" t="n">
-        <v>101837</v>
+        <v>101839</v>
       </c>
       <c r="K67" t="inlineStr">
         <is>
@@ -5188,7 +5188,7 @@
       </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>{'rate': 4.946554400816206e-06, 'diff': -3.58, 'diff7d': 12.18, 'ts': 1675054200, 'marketCapUsd': 158288.95131151724, 'availableSupply': 31999840391, 'volume24h': 909.2925643313138, 'volDiff1': -85.75251581358268, 'volDiff7': 12.868815114161663, 'volDiff30': -35.39856480323279, 'bid': 9.83e-06, 'currency': 'USD'}</t>
+          <t>{'rate': 5.001602494409345e-06, 'diff': 6.69, 'diff7d': 2.06, 'ts': 1675482600, 'marketCapUsd': 160050.48152032652, 'availableSupply': 31999840391, 'volume24h': 1493.44222056373, 'volDiff1': -32.56856416594766, 'volDiff7': -10.285268480443833, 'volDiff30': -20.79242105795649, 'bid': 9.83e-06, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O67" t="n">
@@ -6567,7 +6567,7 @@
       </c>
       <c r="G87" t="inlineStr"/>
       <c r="H87" t="n">
-        <v>1673323767</v>
+        <v>1675441215</v>
       </c>
       <c r="I87" t="n">
         <v>0</v>
@@ -6923,7 +6923,7 @@
       </c>
       <c r="G92" t="inlineStr"/>
       <c r="H92" t="n">
-        <v>1674978038</v>
+        <v>1675273430</v>
       </c>
       <c r="I92" t="n">
         <v>0</v>
@@ -7003,13 +7003,13 @@
         </is>
       </c>
       <c r="H93" t="n">
-        <v>1675018868</v>
+        <v>1675476013</v>
       </c>
       <c r="I93" t="n">
         <v>56161</v>
       </c>
       <c r="J93" t="n">
-        <v>179060</v>
+        <v>179054</v>
       </c>
       <c r="K93" t="inlineStr">
         <is>
@@ -7106,7 +7106,7 @@
       </c>
       <c r="N94" t="inlineStr">
         <is>
-          <t>{'rate': 8.193260474620602e-05, 'diff': 2.66, 'diff7d': 0.27, 'ts': 1675054200, 'marketCapUsd': 64519.49667411873, 'availableSupply': 787470346.80484, 'volume24h': 0, 'volDiff30': -100, 'volDiff1': -100, 'volDiff7': -100, 'bid': 2.861e-05, 'currency': 'USD'}</t>
+          <t>{'rate': 8.27348650555258e-05, 'diff': 0.82, 'diff7d': 3.49, 'ts': 1675482600, 'marketCapUsd': 65151.252878126536, 'availableSupply': 787470346.80484, 'volume24h': 0, 'volDiff30': -100, 'volDiff1': -100, 'volDiff7': -100, 'bid': 2.861e-05, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O94" t="n">
@@ -7433,13 +7433,13 @@
         </is>
       </c>
       <c r="H99" t="n">
-        <v>1675033975</v>
+        <v>1675482059</v>
       </c>
       <c r="I99" t="n">
         <v>0</v>
       </c>
       <c r="J99" t="n">
-        <v>27057</v>
+        <v>27070</v>
       </c>
       <c r="K99" t="inlineStr">
         <is>
@@ -7456,7 +7456,7 @@
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>{'rate': 0.027417305442815645, 'diff': 2.67, 'diff7d': 5.92, 'ts': 1675055760, 'marketCapUsd': 18538403.339014217, 'availableSupply': 676157012.5, 'volume24h': 5665911.13664025, 'volDiff1': 40.43083552870536, 'volDiff7': -42.92108624328881, 'volDiff30': 101.72656018660967, 'diff30d': 40.017053836755764, 'bid': 0.050358, 'currency': 'USD'}</t>
+          <t>{'rate': 0.029564524019418642, 'diff': 4.66, 'diff7d': 11.39, 'ts': 1675485960, 'marketCapUsd': 19990260.2369546, 'availableSupply': 676157012.5, 'volume24h': 4942375.79270252, 'volDiff1': 29.522329063914185, 'volDiff7': 131.41428727181105, 'volDiff30': 162.60139871758474, 'diff30d': 48.712960683961626, 'bid': 0.050358, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O99" t="n">
@@ -7710,18 +7710,18 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>58103059721878646760</t>
+          <t>58122000553844076917</t>
         </is>
       </c>
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="n">
-        <v>1675055238</v>
+        <v>1675485031</v>
       </c>
       <c r="I103" t="n">
-        <v>1124068</v>
+        <v>1127704</v>
       </c>
       <c r="J103" t="n">
-        <v>316264</v>
+        <v>316862</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
@@ -7738,7 +7738,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>{'rate': 0.02751803783954752, 'diff': 3.54, 'diff7d': 16.89, 'ts': 1675055760, 'marketCapUsd': 4771932507.495313, 'availableSupply': 173411074413.06497, 'volume24h': 3765773.64523507, 'volDiff1': 4.210151509565833, 'volDiff7': -41.096574796243914, 'volDiff30': 49.745760897099416, 'diff30d': 44.49719634828767, 'bid': 0.163126, 'currency': 'USD'}</t>
+          <t>{'rate': 0.0403641542549462, 'diff': 29.85, 'diff7d': 48.59, 'ts': 1675485960, 'marketCapUsd': 6999591357.124909, 'availableSupply': 173411074413.06497, 'volume24h': 20017596.52064345, 'volDiff1': 42.40680655875701, 'volDiff7': 108.1425204393554, 'volDiff30': 102.41378813236187, 'diff30d': 111.40068050299345, 'bid': 0.163126, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O103" t="n">
@@ -8004,18 +8004,18 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>55025722253035414370768788</t>
+          <t>55134176939240971981157050</t>
         </is>
       </c>
       <c r="G107" t="inlineStr"/>
       <c r="H107" t="n">
-        <v>1675054740</v>
+        <v>1675485359</v>
       </c>
       <c r="I107" t="n">
-        <v>19356</v>
+        <v>19600</v>
       </c>
       <c r="J107" t="n">
-        <v>45113</v>
+        <v>45143</v>
       </c>
       <c r="K107" t="inlineStr">
         <is>
@@ -8032,7 +8032,7 @@
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>{'rate': 7.053705937350039, 'diff': 1.91, 'diff7d': 1.59, 'ts': 1675055760, 'marketCapUsd': 330237078.8206684, 'availableSupply': 46817528.50966353, 'volume24h': 10194168.85264899, 'volDiff1': -37.60682063857016, 'volDiff7': 61.10034900074652, 'volDiff30': 9.359874149347803, 'diff30d': 35.5756214051037, 'bid': 13.98, 'currency': 'USD'}</t>
+          <t>{'rate': 7.049824935826758, 'diff': -0.11, 'diff7d': -0.35, 'ts': 1675485960, 'marketCapUsd': 331028537.9814537, 'availableSupply': 46955568.54173611, 'volume24h': 8085085.75678492, 'volDiff1': -31.807981253815868, 'volDiff7': 19.41263087132144, 'volDiff30': 80.37511081676018, 'diff30d': 29.504460638618184, 'bid': 13.98, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O107" t="n">
@@ -8440,7 +8440,7 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>32294334767299762</t>
+          <t>32284517903064882</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
@@ -8449,13 +8449,13 @@
         </is>
       </c>
       <c r="H113" t="n">
-        <v>1675055458</v>
+        <v>1675485222</v>
       </c>
       <c r="I113" t="n">
         <v>1</v>
       </c>
       <c r="J113" t="n">
-        <v>4040797</v>
+        <v>4068099</v>
       </c>
       <c r="K113" t="inlineStr">
         <is>
@@ -8472,7 +8472,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>{'rate': 1.0001208134501682, 'diff': -0.01, 'diff7d': 0, 'ts': 1675055460, 'marketCapUsd': 67784223024.37035, 'availableSupply': 67776034767.77134, 'volume24h': 31898898392.93769, 'volDiff1': 22.998061275779307, 'volDiff7': 7.966133644892963, 'volDiff30': 38.98935874209192, 'diff30d': 0.04248746278847193, 'bid': 1.002, 'currency': 'USD'}</t>
+          <t>{'rate': 1.0001169236180185, 'diff': -0.01, 'diff7d': -0.01, 'ts': 1675485660, 'marketCapUsd': 68036551453.65559, 'availableSupply': 68028597303.930084, 'volume24h': 35631756943.553825, 'volDiff1': -15.983041907330033, 'volDiff7': 10.255899789421989, 'volDiff30': 65.03392213845763, 'diff30d': 0.0306959435933436, 'bid': 1.002, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O113" t="n">
@@ -8673,13 +8673,13 @@
       </c>
       <c r="G116" t="inlineStr"/>
       <c r="H116" t="n">
-        <v>1675055305</v>
+        <v>1675485433</v>
       </c>
       <c r="I116" t="n">
         <v>19</v>
       </c>
       <c r="J116" t="n">
-        <v>165587</v>
+        <v>165553</v>
       </c>
       <c r="K116" t="inlineStr">
         <is>
@@ -8696,7 +8696,7 @@
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>{'rate': 0.32195254277921087, 'diff': 1.53, 'diff7d': 12.5, 'ts': 1675055760, 'marketCapUsd': 428239877.21814644, 'availableSupply': 1330133545.5263836, 'volume24h': 39573054.42978527, 'volDiff1': -8.606111249696752, 'volDiff7': 25.725840657694746, 'volDiff30': 120.91018908093773, 'diff30d': 70.57917286744694, 'bid': 0.81468, 'currency': 'USD'}</t>
+          <t>{'rate': 0.404398612214396, 'diff': -0.59, 'diff7d': 26.9, 'ts': 1675485960, 'marketCapUsd': 537904159.8706837, 'availableSupply': 1330133545.5263836, 'volume24h': 83306622.22655597, 'volDiff1': -57.67062261182398, 'volDiff7': 95.8670584081608, 'volDiff30': 303.6763459902351, 'diff30d': 103.4648608182338, 'bid': 0.81468, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O116" t="n">
@@ -9311,7 +9311,7 @@
       </c>
       <c r="G125" t="inlineStr"/>
       <c r="H125" t="n">
-        <v>1674899445</v>
+        <v>1675389100</v>
       </c>
       <c r="I125" t="n">
         <v>1</v>
@@ -9379,13 +9379,13 @@
         </is>
       </c>
       <c r="H126" t="n">
-        <v>1675054435</v>
+        <v>1675479900</v>
       </c>
       <c r="I126" t="n">
         <v>39</v>
       </c>
       <c r="J126" t="n">
-        <v>42639</v>
+        <v>42660</v>
       </c>
       <c r="K126" t="inlineStr">
         <is>
@@ -9402,7 +9402,7 @@
       </c>
       <c r="N126" t="inlineStr">
         <is>
-          <t>{'rate': 0.11307987288569732, 'diff': 1.72, 'diff7d': 3.19, 'ts': 1675055760, 'marketCapUsd': 113060685.04505457, 'availableSupply': 999830316.0398655, 'volume24h': 3545252.36928746, 'volDiff1': 33.25594118336198, 'volDiff7': -42.74995204866653, 'volDiff30': 14.43936416915328, 'diff30d': 32.56275360778332, 'bid': 0.199662, 'currency': 'USD'}</t>
+          <t>{'rate': 0.10959211234475345, 'diff': 2.06, 'diff7d': -2.11, 'ts': 1675485960, 'marketCapUsd': 109573516.32113129, 'availableSupply': 999830316.0398655, 'volume24h': 3315153.8851935, 'volDiff1': -5.022267015964346, 'volDiff7': -53.15892301662546, 'volDiff30': 30.850842816423267, 'diff30d': 26.54451321307411, 'bid': 0.199662, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O126" t="n">
@@ -9448,7 +9448,7 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>297574806517519794239794008</t>
+          <t>297726294349683794239794008</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
@@ -9457,13 +9457,13 @@
         </is>
       </c>
       <c r="H127" t="n">
-        <v>1675055571</v>
+        <v>1675485292</v>
       </c>
       <c r="I127" t="n">
-        <v>214484</v>
+        <v>214509</v>
       </c>
       <c r="J127" t="n">
-        <v>46328</v>
+        <v>46431</v>
       </c>
       <c r="K127" t="inlineStr"/>
       <c r="L127" t="inlineStr"/>
@@ -9472,7 +9472,7 @@
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>{'rate': 0.022177306776386397, 'diff': -1.09, 'diff7d': -4.11, 'ts': 1675055820, 'marketCapUsd': 217378225.14488208, 'availableSupply': 9801831545.04309, 'volume24h': 9528273.97820652, 'volDiff1': -16.303497440618813, 'volDiff7': -40.5231033152001, 'volDiff30': -37.050961501347736, 'diff30d': 10.844148254344702, 'bid': 0.989608, 'currency': 'USD'}</t>
+          <t>{'rate': 0.036757386874964895, 'diff': 23.96, 'diff7d': 65.63, 'ts': 1675486080, 'marketCapUsd': 360249931.2908832, 'availableSupply': 9800749234.876812, 'volume24h': 370360248.0940502, 'volDiff1': 322.99997720267584, 'volDiff7': 485.32835344783985, 'volDiff30': 44.231138677042594, 'diff30d': 79.62881790169806, 'bid': 0.989608, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O127" t="n">
@@ -9531,13 +9531,13 @@
         </is>
       </c>
       <c r="H128" t="n">
-        <v>1675054853</v>
+        <v>1675485355</v>
       </c>
       <c r="I128" t="n">
         <v>28513</v>
       </c>
       <c r="J128" t="n">
-        <v>25267</v>
+        <v>25317</v>
       </c>
       <c r="K128" t="inlineStr">
         <is>
@@ -9549,10 +9549,12 @@
           <t>/images/MIR09a3ecaf.png</t>
         </is>
       </c>
-      <c r="M128" t="inlineStr"/>
+      <c r="M128" t="n">
+        <v>0</v>
+      </c>
       <c r="N128" t="inlineStr">
         <is>
-          <t>{'rate': 0.16608847866580176, 'diff': -0.26, 'diff7d': 2.9, 'ts': 1675055760, 'marketCapUsd': 12912163.437390119, 'availableSupply': 77742679.932493, 'volume24h': 10126906.7497994, 'volDiff1': -22.331277381575205, 'volDiff7': -10.263690521815846, 'volDiff30': -11.700549875713293, 'diff30d': 22.136613933898275, 'bid': 1.13, 'currency': 'USD'}</t>
+          <t>{'rate': 0.18180823256924172, 'diff': 7.17, 'diff7d': 13.57, 'ts': 1675485960, 'marketCapUsd': 14134259.23372281, 'availableSupply': 77742679.932493, 'volume24h': 47252376.3102048, 'volDiff1': 198.73761960707998, 'volDiff7': 96.090227589107, 'volDiff30': -4.33669052666707, 'diff30d': 33.65080652006873, 'bid': 1.13, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O128" t="n">
@@ -9611,7 +9613,7 @@
         </is>
       </c>
       <c r="H129" t="n">
-        <v>1674298386</v>
+        <v>1675363345</v>
       </c>
       <c r="I129" t="n">
         <v>2</v>
@@ -9689,7 +9691,7 @@
         </is>
       </c>
       <c r="H130" t="n">
-        <v>1674737888</v>
+        <v>1675130545</v>
       </c>
       <c r="I130" t="n">
         <v>839</v>
@@ -9829,13 +9831,13 @@
       </c>
       <c r="G132" t="inlineStr"/>
       <c r="H132" t="n">
-        <v>1675055288</v>
+        <v>1675483063</v>
       </c>
       <c r="I132" t="n">
         <v>4</v>
       </c>
       <c r="J132" t="n">
-        <v>99331</v>
+        <v>99361</v>
       </c>
       <c r="K132" t="inlineStr">
         <is>
@@ -9852,7 +9854,7 @@
       </c>
       <c r="N132" t="inlineStr">
         <is>
-          <t>{'rate': 0.009527082358817551, 'diff': 4.1, 'diff7d': 5.07, 'ts': 1675054200, 'marketCapUsd': 10752574.898680855, 'availableSupply': 1128632512.4217153, 'volume24h': 224.64446218, 'volDiff1': -4.92463770414038, 'volDiff7': -35.33032944731961, 'volDiff30': 12.90006114592866, 'bid': 0.01610347, 'currency': 'USD'}</t>
+          <t>{'rate': 0.009738731520595841, 'diff': 2.61, 'diff7d': 6.7, 'ts': 1675482600, 'marketCapUsd': 10991449.023890635, 'availableSupply': 1128632512.4217153, 'volume24h': 170.5349966, 'volDiff1': -15.067278178512993, 'volDiff7': 1.726424649061073, 'volDiff30': 11.889882484291988, 'bid': 0.01610347, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O132" t="n">
@@ -10163,13 +10165,13 @@
       </c>
       <c r="G137" t="inlineStr"/>
       <c r="H137" t="n">
-        <v>1675020439</v>
+        <v>1675363885</v>
       </c>
       <c r="I137" t="n">
         <v>2</v>
       </c>
       <c r="J137" t="n">
-        <v>4830</v>
+        <v>4831</v>
       </c>
       <c r="K137" t="inlineStr"/>
       <c r="L137" t="inlineStr"/>
@@ -10495,13 +10497,13 @@
       </c>
       <c r="G142" t="inlineStr"/>
       <c r="H142" t="n">
-        <v>1675019455</v>
+        <v>1675384650</v>
       </c>
       <c r="I142" t="n">
         <v>70</v>
       </c>
       <c r="J142" t="n">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="K142" t="inlineStr">
         <is>
@@ -10518,7 +10520,7 @@
       </c>
       <c r="N142" t="inlineStr">
         <is>
-          <t>{'rate': 1.00624726516949, 'diff': 0.36, 'diff7d': 0.08, 'ts': 1675055460, 'marketCapUsd': 4779603.7315311795, 'availableSupply': 0, 'volume24h': 41459.28958142, 'volDiff1': 14.172965038456795, 'volDiff7': 12.180632087086153, 'volDiff30': -1.424682099083725, 'bid': 2.59, 'currency': 'USD'}</t>
+          <t>{'rate': 1.0112482249778871, 'diff': 1.49, 'diff7d': -0.15, 'ts': 1675485660, 'marketCapUsd': 4747888.507345039, 'availableSupply': 0, 'volume24h': 36775.37319880154, 'volDiff1': -7.300251001901557, 'volDiff7': 6.139543076956571, 'volDiff30': 9.271930814553755, 'bid': 2.59, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O142" t="n">
@@ -10628,7 +10630,7 @@
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>247218846537743114147285206</t>
+          <t>247309633035212496801621367</t>
         </is>
       </c>
       <c r="G144" t="inlineStr">
@@ -10637,13 +10639,13 @@
         </is>
       </c>
       <c r="H144" t="n">
-        <v>1675055612</v>
+        <v>1675485818</v>
       </c>
       <c r="I144" t="n">
-        <v>872197</v>
+        <v>872727</v>
       </c>
       <c r="J144" t="n">
-        <v>112005</v>
+        <v>112245</v>
       </c>
       <c r="K144" t="inlineStr">
         <is>
@@ -10660,7 +10662,7 @@
       </c>
       <c r="N144" t="inlineStr">
         <is>
-          <t>{'rate': 1.325250007891281, 'diff': 1.09, 'diff7d': -3.02, 'ts': 1675055760, 'marketCapUsd': 294546583.9968954, 'availableSupply': 222257372, 'volume24h': 42009332.53416287, 'volDiff1': 4.2184536020911025, 'volDiff7': -20.033212584339438, 'volDiff30': 38.60881327232474, 'diff30d': 43.062609458626895, 'bid': 2.87, 'currency': 'USD'}</t>
+          <t>{'rate': 1.5309747285443547, 'diff': 0.61, 'diff7d': 13.04, 'ts': 1675485960, 'marketCapUsd': 340270419.76468164, 'availableSupply': 222257372, 'volume24h': 127462282.51774907, 'volDiff1': -23.25390319400924, 'volDiff7': 41.30131174470691, 'volDiff30': 88.55550318914118, 'diff30d': 55.17547092154612, 'bid': 2.87, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O144" t="n">
@@ -10787,13 +10789,13 @@
       </c>
       <c r="G146" t="inlineStr"/>
       <c r="H146" t="n">
-        <v>1675055663</v>
+        <v>1675479554</v>
       </c>
       <c r="I146" t="n">
         <v>1</v>
       </c>
       <c r="J146" t="n">
-        <v>3492</v>
+        <v>3484</v>
       </c>
       <c r="K146" t="inlineStr">
         <is>
@@ -10805,10 +10807,12 @@
           <t>/images/FOLDd084944d.png</t>
         </is>
       </c>
-      <c r="M146" t="inlineStr"/>
+      <c r="M146" t="n">
+        <v>0</v>
+      </c>
       <c r="N146" t="inlineStr">
         <is>
-          <t>{'rate': 26.034286279237953, 'diff': 7.37, 'diff7d': -8.95, 'ts': 1675055760, 'marketCapUsd': 40347653.44651634, 'availableSupply': 0, 'volume24h': 2070599.93909221, 'volDiff1': 148.2260348535345, 'volDiff7': 54.735754178703615, 'volDiff30': 195.34104079783629, 'diff30d': 109.28075595414981, 'bid': 12.29, 'currency': 'USD'}</t>
+          <t>{'rate': 27.821997837727004, 'diff': -1.94, 'diff7d': 5.36, 'ts': 1675485960, 'marketCapUsd': 42161184.54602267, 'availableSupply': 0, 'volume24h': 1587995.57124498, 'volDiff1': -18.445437440437743, 'volDiff7': 8.06871120969413, 'volDiff30': 354.46340424861023, 'diff30d': 114.18179900711718, 'bid': 12.29, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O146" t="n">
@@ -11259,13 +11263,13 @@
       </c>
       <c r="G153" t="inlineStr"/>
       <c r="H153" t="n">
-        <v>1675054943</v>
+        <v>1675485802</v>
       </c>
       <c r="I153" t="n">
         <v>2783</v>
       </c>
       <c r="J153" t="n">
-        <v>1291901</v>
+        <v>1296491</v>
       </c>
       <c r="K153" t="inlineStr">
         <is>
@@ -11282,7 +11286,7 @@
       </c>
       <c r="N153" t="inlineStr">
         <is>
-          <t>{'rate': 1.2033582125333629e-05, 'diff': 0.69, 'diff7d': -0.59, 'ts': 1675055760, 'marketCapUsd': 6607198058.362941, 'availableSupply': 549063278876301.94, 'volume24h': 215394700.03588519, 'volDiff1': -27.625115063910798, 'volDiff7': -47.72873085899002, 'volDiff30': 191.11218744491418, 'diff30d': 48.68039470086035, 'bid': 2.263e-05, 'currency': 'USD'}</t>
+          <t>{'rate': 1.4101384890419376e-05, 'diff': 11.74, 'diff7d': 19.15, 'ts': 1675485960, 'marketCapUsd': 7742552624.630404, 'availableSupply': 549063278876301.94, 'volume24h': 1036097732.7701277, 'volDiff1': 93.82004160666119, 'volDiff7': 62.18339803877723, 'volDiff30': 282.3044850751299, 'diff30d': 66.12115877324388, 'bid': 2.263e-05, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O153" t="n">
@@ -11333,13 +11337,13 @@
       </c>
       <c r="G154" t="inlineStr"/>
       <c r="H154" t="n">
-        <v>1675054828</v>
+        <v>1675485072</v>
       </c>
       <c r="I154" t="n">
         <v>1</v>
       </c>
       <c r="J154" t="n">
-        <v>12819</v>
+        <v>12952</v>
       </c>
       <c r="K154" t="inlineStr">
         <is>
@@ -11356,7 +11360,7 @@
       </c>
       <c r="N154" t="inlineStr">
         <is>
-          <t>{'rate': 3.0862398969086957, 'diff': -1.28, 'diff7d': -7.04, 'ts': 1675055760, 'marketCapUsd': 210481560.96917304, 'availableSupply': 68200000, 'volume24h': 62658601.11056202, 'volDiff1': -22.21969012399437, 'volDiff7': -26.588722213431467, 'volDiff30': 4.3409348687153795, 'diff30d': 49.88616818479227, 'bid': 4.57, 'currency': 'USD'}</t>
+          <t>{'rate': 4.761274675656645, 'diff': -3.39, 'diff7d': 45.93, 'ts': 1675485960, 'marketCapUsd': 324718932.87978315, 'availableSupply': 68200000, 'volume24h': 244227184.57808354, 'volDiff1': -10.068982405665707, 'volDiff7': 199.96539298007804, 'volDiff30': 95.83593903105128, 'diff30d': 106.02171191555536, 'bid': 4.57, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O154" t="n">
@@ -11402,7 +11406,7 @@
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>193953403405706536911463221</t>
+          <t>193953352884211389870161728</t>
         </is>
       </c>
       <c r="G155" t="inlineStr">
@@ -11411,13 +11415,13 @@
         </is>
       </c>
       <c r="H155" t="n">
-        <v>1675047447</v>
+        <v>1675384626</v>
       </c>
       <c r="I155" t="n">
-        <v>156761</v>
+        <v>156765</v>
       </c>
       <c r="J155" t="n">
-        <v>30024</v>
+        <v>30025</v>
       </c>
       <c r="K155" t="inlineStr">
         <is>
@@ -11434,11 +11438,11 @@
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>{'rate': 0.28813802350060735, 'diff': 91.04, 'diff7d': -90.15, 'ts': 1654789260, 'marketCapUsd': 245096369.2157965, 'availableSupply': 0, 'volume24h': 1556540.1873397797, 'volDiff1': 20710.816313813164, 'volDiff7': -100, 'volDiff30': -100, 'diff30d': -88.50367917609971, 'bid': 2.78, 'currency': 'USD'}</t>
+          <t>{'rate': 0.28813802350060735, 'diff': 91.04, 'diff7d': -90.15, 'ts': 1654789260, 'marketCapUsd': 245096369.2157965, 'availableSupply': 0, 'volume24h': 1556540.1873397797, 'volDiff1': 1958.2321142307246, 'volDiff7': 2.7212464425504095, 'volDiff30': -67.43441801163681, 'diff30d': -88.50367917609971, 'bid': 2.78, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O155" t="n">
-        <v>3538619031649</v>
+        <v>3538621108679</v>
       </c>
       <c r="P155" t="n">
         <v>0</v>
@@ -11448,7 +11452,7 @@
       </c>
       <c r="R155" t="inlineStr">
         <is>
-          <t>3538619031649</t>
+          <t>3538621108679</t>
         </is>
       </c>
       <c r="S155" t="inlineStr"/>
@@ -11625,13 +11629,13 @@
         </is>
       </c>
       <c r="H158" t="n">
-        <v>1675055268</v>
+        <v>1675463256</v>
       </c>
       <c r="I158" t="n">
         <v>168</v>
       </c>
       <c r="J158" t="n">
-        <v>7049</v>
+        <v>7056</v>
       </c>
       <c r="K158" t="inlineStr">
         <is>
@@ -11643,10 +11647,12 @@
           <t>/images/AAA8c6bf16c.png</t>
         </is>
       </c>
-      <c r="M158" t="inlineStr"/>
+      <c r="M158" t="n">
+        <v>0</v>
+      </c>
       <c r="N158" t="inlineStr">
         <is>
-          <t>{'rate': 1.0187629358820485e-05, 'diff': -8.93, 'diff7d': -0.26, 'ts': 1675055460, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 137106.73560301, 'volDiff1': 12.33530898394875, 'volDiff7': 6.782930734244658, 'volDiff30': 10.57710380176178, 'diff30d': -42.37306409848739, 'bid': 0.00010443, 'currency': 'USD'}</t>
+          <t>{'rate': 9.50212208911753e-06, 'diff': -10.48, 'diff7d': -18.19, 'ts': 1675485660, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 112138.43881558, 'volDiff1': -4.877932729346213, 'volDiff7': 9.87713491264364, 'volDiff30': 8.188180505031767, 'diff30d': -42.37306409848739, 'bid': 0.00010443, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O158" t="n">
@@ -12301,13 +12307,13 @@
       </c>
       <c r="G168" t="inlineStr"/>
       <c r="H168" t="n">
-        <v>1675033041</v>
+        <v>1675484049</v>
       </c>
       <c r="I168" t="n">
         <v>1</v>
       </c>
       <c r="J168" t="n">
-        <v>1841</v>
+        <v>1839</v>
       </c>
       <c r="K168" t="inlineStr">
         <is>
@@ -12324,7 +12330,7 @@
       </c>
       <c r="N168" t="inlineStr">
         <is>
-          <t>{'rate': 4.557264748215605e-06, 'diff': -8.61, 'diff7d': -3.03, 'ts': 1675054200, 'marketCapUsd': 144050.05385239332, 'availableSupply': 0, 'volume24h': 103.2572735279714, 'volDiff1': -86.52543141950594, 'volDiff7': 42.31243431329372, 'volDiff30': 20.72146285667536, 'bid': 1.345e-05, 'currency': 'USD'}</t>
+          <t>{'rate': 2.9527134302068606e-06, 'diff': -28.67, 'diff7d': -41.14, 'ts': 1675482600, 'marketCapUsd': 95287.85542859277, 'availableSupply': 0, 'volume24h': 426.67000733, 'volDiff1': 1064.1746448294678, 'volDiff7': 73.2519761098188, 'volDiff30': 187.04726167792643, 'bid': 1.345e-05, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O168" t="n">
@@ -12370,18 +12376,18 @@
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>954000000000000000000</t>
+          <t>953000000000000000000</t>
         </is>
       </c>
       <c r="G169" t="inlineStr"/>
       <c r="H169" t="n">
-        <v>1674993806</v>
+        <v>1675275484</v>
       </c>
       <c r="I169" t="n">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="J169" t="n">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K169" t="inlineStr"/>
       <c r="L169" t="inlineStr"/>
@@ -12503,13 +12509,13 @@
       </c>
       <c r="G171" t="inlineStr"/>
       <c r="H171" t="n">
-        <v>1675055038</v>
+        <v>1675481506</v>
       </c>
       <c r="I171" t="n">
         <v>9</v>
       </c>
       <c r="J171" t="n">
-        <v>8923</v>
+        <v>8925</v>
       </c>
       <c r="K171" t="inlineStr">
         <is>
@@ -12521,10 +12527,12 @@
           <t>/images/TORN77777fed.jpg</t>
         </is>
       </c>
-      <c r="M171" t="inlineStr"/>
+      <c r="M171" t="n">
+        <v>0</v>
+      </c>
       <c r="N171" t="inlineStr">
         <is>
-          <t>{'rate': 6.229109322407132, 'diff': 4.75, 'diff7d': 14.13, 'ts': 1675055760, 'marketCapUsd': 6850741.472803226, 'availableSupply': 1099794.70871702, 'volume24h': 5421234.24075116, 'volDiff1': 71.59105827487525, 'volDiff7': 20.30489810985179, 'volDiff30': 10.998403282823006, 'diff30d': 57.43035313054094, 'bid': 51.86, 'currency': 'USD'}</t>
+          <t>{'rate': 6.97238050416101, 'diff': 11.41, 'diff7d': 16.53, 'ts': 1675485960, 'marketCapUsd': 7668187.185637987, 'availableSupply': 1099794.70871702, 'volume24h': 17553348.86495766, 'volDiff1': 88.88538138577374, 'volDiff7': 4.644258205503135, 'volDiff30': 78.28110981591846, 'diff30d': 72.70080158287519, 'bid': 51.86, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O171" t="n">
@@ -12647,13 +12655,13 @@
         </is>
       </c>
       <c r="H173" t="n">
-        <v>1675054822</v>
+        <v>1675485320</v>
       </c>
       <c r="I173" t="n">
         <v>1</v>
       </c>
       <c r="J173" t="n">
-        <v>35204</v>
+        <v>35632</v>
       </c>
       <c r="K173" t="inlineStr">
         <is>
@@ -12665,10 +12673,12 @@
           <t>/images/DYDX92d6c1e3.jpg</t>
         </is>
       </c>
-      <c r="M173" t="inlineStr"/>
+      <c r="M173" t="n">
+        <v>0</v>
+      </c>
       <c r="N173" t="inlineStr">
         <is>
-          <t>{'rate': 2.330108304240725, 'diff': 0.35, 'diff7d': 31.02, 'ts': 1675055760, 'marketCapUsd': 364093808.6262837, 'availableSupply': 156256174, 'volume24h': 133997454.19585787, 'volDiff1': 3.5124144822235053, 'volDiff7': 137.76224290283116, 'volDiff30': 78.16550077318911, 'diff30d': 117.66699912675631, 'bid': 4.27, 'currency': 'USD'}</t>
+          <t>{'rate': 3.0985868465262887, 'diff': -3.4, 'diff7d': 27.16, 'ts': 1675485960, 'marketCapUsd': 484173325.44492304, 'availableSupply': 156256174, 'volume24h': 203338491.81140223, 'volDiff1': -31.63849472905339, 'volDiff7': 71.03491500433967, 'volDiff30': 190.3934973142807, 'diff30d': 159.65092975165913, 'bid': 4.27, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O173" t="n">
@@ -12787,13 +12797,13 @@
         </is>
       </c>
       <c r="H175" t="n">
-        <v>1675035032</v>
+        <v>1675483907</v>
       </c>
       <c r="I175" t="n">
         <v>0</v>
       </c>
       <c r="J175" t="n">
-        <v>7852</v>
+        <v>7855</v>
       </c>
       <c r="K175" t="inlineStr">
         <is>
@@ -12810,7 +12820,7 @@
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>{'rate': 0.23270114152910476, 'diff': 1.06, 'diff7d': -1.28, 'ts': 1675055460, 'marketCapUsd': 2258771.805537638, 'availableSupply': 9706750, 'volume24h': 113864.61427837, 'volDiff1': 9.195654137322478, 'volDiff7': 9.60875503361072, 'volDiff30': 23.314620891773615, 'bid': 0.695983, 'currency': 'USD'}</t>
+          <t>{'rate': 0.19485251684377972, 'diff': 3.79, 'diff7d': -12.38, 'ts': 1675485660, 'marketCapUsd': 1891384.6678733588, 'availableSupply': 9706750, 'volume24h': 115605.81169949, 'volDiff1': 22.012471789048064, 'volDiff7': 10.14360000873404, 'volDiff30': 30.18614957142819, 'bid': 0.695983, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O175" t="n">
@@ -12865,13 +12875,13 @@
         </is>
       </c>
       <c r="H176" t="n">
-        <v>1675042370</v>
+        <v>1675484479</v>
       </c>
       <c r="I176" t="n">
         <v>6</v>
       </c>
       <c r="J176" t="n">
-        <v>9571</v>
+        <v>9550</v>
       </c>
       <c r="K176" t="inlineStr">
         <is>
@@ -12945,13 +12955,13 @@
       </c>
       <c r="G177" t="inlineStr"/>
       <c r="H177" t="n">
-        <v>1675048082</v>
+        <v>1675483570</v>
       </c>
       <c r="I177" t="n">
         <v>1</v>
       </c>
       <c r="J177" t="n">
-        <v>5760</v>
+        <v>5772</v>
       </c>
       <c r="K177" t="inlineStr">
         <is>
@@ -12968,7 +12978,7 @@
       </c>
       <c r="N177" t="inlineStr">
         <is>
-          <t>{'rate': 4.5854101353797756e-05, 'diff': 3.13, 'diff7d': 6.68, 'ts': 1675054200, 'marketCapUsd': 8809.108312532926, 'availableSupply': 192111677.09, 'volume24h': 805.8812989, 'volDiff1': 95.59434462198138, 'volDiff7': -93.89015724364018, 'volDiff30': 222.4739324916659, 'diff30d': -97.97570220719227, 'bid': 0.03378307, 'currency': 'USD'}</t>
+          <t>{'rate': 5.138353124739471e-05, 'diff': 2.57, 'diff7d': 17.39, 'ts': 1675482600, 'marketCapUsd': 9871.376362743416, 'availableSupply': 192111677.09, 'volume24h': 356.95330553, 'volDiff1': -90.89673054163887, 'volDiff7': 462.75330938225693, 'volDiff30': 181.5934639686713, 'diff30d': -97.97570220719227, 'bid': 0.03378307, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O177" t="n">
@@ -13023,13 +13033,13 @@
         </is>
       </c>
       <c r="H178" t="n">
-        <v>1675020195</v>
+        <v>1675484130</v>
       </c>
       <c r="I178" t="n">
         <v>1</v>
       </c>
       <c r="J178" t="n">
-        <v>13174</v>
+        <v>13204</v>
       </c>
       <c r="K178" t="inlineStr">
         <is>
@@ -13046,7 +13056,7 @@
       </c>
       <c r="N178" t="inlineStr">
         <is>
-          <t>{'rate': 5.1562179751886736e-06, 'diff': 1.1, 'diff7d': 6.73, 'ts': 1675055460, 'marketCapUsd': 2222053.001947851, 'availableSupply': 0, 'volume24h': 790100.00397669, 'volDiff1': 116.893571870974, 'volDiff7': 28.72152232045164, 'volDiff30': 131.54277620388763, 'diff30d': 23.88693472069218, 'bid': 1.602e-05, 'currency': 'USD'}</t>
+          <t>{'rate': 1.5179918423678729e-05, 'diff': -3.47, 'diff7d': 179.06, 'ts': 1675485960, 'marketCapUsd': 6020006.602495179, 'availableSupply': 0, 'volume24h': 4174207.83496092, 'volDiff1': -53.47238710105694, 'volDiff7': 440.1149578751531, 'volDiff30': 390.6406030624262, 'diff30d': 324.4404398243584, 'bid': 1.602e-05, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O178" t="n">
@@ -13569,13 +13579,13 @@
         </is>
       </c>
       <c r="H186" t="n">
-        <v>1675055355</v>
+        <v>1675485573</v>
       </c>
       <c r="I186" t="n">
         <v>2</v>
       </c>
       <c r="J186" t="n">
-        <v>64310</v>
+        <v>64222</v>
       </c>
       <c r="K186" t="inlineStr">
         <is>
@@ -13592,7 +13602,7 @@
       </c>
       <c r="N186" t="inlineStr">
         <is>
-          <t>{'rate': 15.890107808983771, 'diff': -0.61, 'diff7d': 6.76, 'ts': 1675055760, 'marketCapUsd': 321693041.19681233, 'availableSupply': 20244862.09054775, 'volume24h': 36575540.47609901, 'volDiff1': -1.3938867187430048, 'volDiff7': 36.36648631613258, 'volDiff30': 149.49014893643871, 'diff30d': 48.45311712496013, 'bid': 18.22, 'currency': 'USD'}</t>
+          <t>{'rate': 16.202651992070322, 'diff': 0.78, 'diff7d': -3.56, 'ts': 1675485960, 'marketCapUsd': 328020455.08060247, 'availableSupply': 20244862.09054775, 'volume24h': 48335957.26698524, 'volDiff1': -14.341178419487377, 'volDiff7': -24.519926355899727, 'volDiff30': 216.6836955956495, 'diff30d': 39.836678515205335, 'bid': 18.22, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O186" t="n">
@@ -13715,13 +13725,13 @@
         </is>
       </c>
       <c r="H188" t="n">
-        <v>1675055135</v>
+        <v>1675481927</v>
       </c>
       <c r="I188" t="n">
         <v>0</v>
       </c>
       <c r="J188" t="n">
-        <v>5001</v>
+        <v>4989</v>
       </c>
       <c r="K188" t="inlineStr">
         <is>
@@ -13733,10 +13743,12 @@
           <t>/images/NCRdb5c3c46.png</t>
         </is>
       </c>
-      <c r="M188" t="inlineStr"/>
+      <c r="M188" t="n">
+        <v>0</v>
+      </c>
       <c r="N188" t="inlineStr">
         <is>
-          <t>{'rate': 0.11982450541323648, 'diff': 16.39, 'diff7d': 5.23, 'ts': 1675055460, 'marketCapUsd': 4842350.681318367, 'availableSupply': 0, 'volume24h': 54657.050317182395, 'volDiff1': 476.6995464086697, 'volDiff7': -49.146071580459015, 'volDiff30': -8.595985619140137, 'diff30d': -82.70311426146176, 'bid': 0.402762, 'currency': 'USD'}</t>
+          <t>{'rate': 0.11171914014924386, 'diff': -0.18, 'diff7d': 6.8, 'ts': 1675482600, 'marketCapUsd': 4545580.936378445, 'availableSupply': 0, 'volume24h': 1465.1526299245784, 'volDiff1': -58.137320145911396, 'volDiff7': -71.42707266775322, 'volDiff30': -8.772144006595681, 'diff30d': -82.70311426146176, 'bid': 0.402762, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O188" t="n">
@@ -14119,13 +14131,13 @@
         </is>
       </c>
       <c r="H194" t="n">
-        <v>1672855408</v>
+        <v>1675425431</v>
       </c>
       <c r="I194" t="n">
         <v>0</v>
       </c>
       <c r="J194" t="n">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="K194" t="inlineStr">
         <is>
@@ -14650,7 +14662,7 @@
       </c>
       <c r="F202" t="inlineStr">
         <is>
-          <t>39875290613469550</t>
+          <t>38884778184049550</t>
         </is>
       </c>
       <c r="G202" t="inlineStr">
@@ -14659,13 +14671,13 @@
         </is>
       </c>
       <c r="H202" t="n">
-        <v>1675055573</v>
+        <v>1675485343</v>
       </c>
       <c r="I202" t="n">
-        <v>319804</v>
+        <v>322371</v>
       </c>
       <c r="J202" t="n">
-        <v>1596461</v>
+        <v>1606494</v>
       </c>
       <c r="K202" t="inlineStr">
         <is>
@@ -14682,7 +14694,7 @@
       </c>
       <c r="N202" t="inlineStr">
         <is>
-          <t>{'rate': 0.9999228672966683, 'diff': -0.01, 'diff7d': -0.01, 'ts': 1675055760, 'marketCapUsd': 43087330788.60382, 'availableSupply': 43090654487.27275, 'volume24h': 2783192632.461068, 'volDiff1': 5.4218976016767755, 'volDiff7': 8.039857034797876, 'volDiff30': 49.142850725464484, 'diff30d': -0.017323469030571914, 'bid': 1.001, 'currency': 'USD'}</t>
+          <t>{'rate': 0.99992463787292, 'diff': -0.02, 'diff7d': -0.01, 'ts': 1675485960, 'marketCapUsd': 41959609610.84966, 'availableSupply': 41962772014.60686, 'volume24h': 3265529322.79822, 'volDiff1': -20.30784648935348, 'volDiff7': 4.941416092745413, 'volDiff30': 70.48602329758552, 'diff30d': -0.006848808093351977, 'bid': 1.001, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O202" t="n">
@@ -16285,13 +16297,13 @@
       </c>
       <c r="G226" t="inlineStr"/>
       <c r="H226" t="n">
-        <v>1674673790</v>
+        <v>1675443369</v>
       </c>
       <c r="I226" t="n">
         <v>0</v>
       </c>
       <c r="J226" t="n">
-        <v>5642</v>
+        <v>5643</v>
       </c>
       <c r="K226" t="inlineStr">
         <is>
@@ -16308,7 +16320,7 @@
       </c>
       <c r="N226" t="inlineStr">
         <is>
-          <t>{'rate': 0.0009001008816689417, 'diff': -0.02, 'diff7d': -0.01, 'ts': 1675054200, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 0.0009001, 'volDiff1': -90.99889999999999, 'volDiff7': -1.690319047618999, 'volDiff30': 2.305315834522247, 'diff30d': -47.733420758138536, 'bid': 0.01063471, 'currency': 'USD'}</t>
+          <t>{'rate': 0.0009001084273082205, 'diff': 0, 'diff7d': -0.01, 'ts': 1675482600, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 0.0009001, 'volDiff1': -90.999, 'volDiff7': -1.095095238095439, 'volDiff30': 2.5943199999998683, 'diff30d': -47.733420758138536, 'bid': 0.01063471, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O226" t="n">
@@ -20142,18 +20154,18 @@
       </c>
       <c r="F283" t="inlineStr">
         <is>
-          <t>2965718473712</t>
+          <t>3007431814585</t>
         </is>
       </c>
       <c r="G283" t="inlineStr"/>
       <c r="H283" t="n">
-        <v>1675047807</v>
+        <v>1675483787</v>
       </c>
       <c r="I283" t="n">
-        <v>110976</v>
+        <v>111752</v>
       </c>
       <c r="J283" t="n">
-        <v>3163</v>
+        <v>3153</v>
       </c>
       <c r="K283" t="inlineStr">
         <is>
@@ -24647,7 +24659,9 @@
       </c>
       <c r="K349" t="inlineStr"/>
       <c r="L349" t="inlineStr"/>
-      <c r="M349" t="inlineStr"/>
+      <c r="M349" t="n">
+        <v>0</v>
+      </c>
       <c r="N349" t="b">
         <v>0</v>
       </c>
@@ -26006,7 +26020,7 @@
       </c>
       <c r="N369" t="inlineStr">
         <is>
-          <t>{'rate': 1.9587060902195004, 'diff': 1.48, 'diff7d': -12.02, 'ts': 1675054200, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 53.935048504340806, 'volDiff1': -96.23826828221891, 'volDiff7': 12.780065032133365, 'volDiff30': -29.264279316217184, 'currency': 'USD'}</t>
+          <t>{'rate': 1.9712135811431237, 'diff': -2.93, 'diff7d': -0.53, 'ts': 1675482600, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 201.75006924, 'volDiff1': 34.048748706023076, 'volDiff7': -56.1946296638883, 'volDiff30': -23.336148386533154, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O369" t="n">
@@ -26121,13 +26135,13 @@
       </c>
       <c r="G371" t="inlineStr"/>
       <c r="H371" t="n">
-        <v>1674738161</v>
+        <v>1675448067</v>
       </c>
       <c r="I371" t="n">
         <v>1</v>
       </c>
       <c r="J371" t="n">
-        <v>2837</v>
+        <v>2838</v>
       </c>
       <c r="K371" t="inlineStr"/>
       <c r="L371" t="inlineStr"/>
@@ -26244,7 +26258,7 @@
       </c>
       <c r="F373" t="inlineStr">
         <is>
-          <t>16864434545339999999985000000</t>
+          <t>16864534545339999999985000000</t>
         </is>
       </c>
       <c r="G373" t="inlineStr">
@@ -26253,13 +26267,13 @@
         </is>
       </c>
       <c r="H373" t="n">
-        <v>1675050274</v>
+        <v>1675483310</v>
       </c>
       <c r="I373" t="n">
-        <v>8323</v>
+        <v>8324</v>
       </c>
       <c r="J373" t="n">
-        <v>6258</v>
+        <v>6254</v>
       </c>
       <c r="K373" t="inlineStr">
         <is>
@@ -26276,7 +26290,7 @@
       </c>
       <c r="N373" t="inlineStr">
         <is>
-          <t>{'rate': 7.024829490997202e-05, 'diff': -3.72, 'diff7d': 15.12, 'ts': 1675055460, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 74530.94971655, 'volDiff1': 15.774787820519435, 'volDiff7': 16.29279789655635, 'volDiff30': -9.704854023027153, 'diff30d': -89.09726477912302, 'bid': 0.00034117, 'currency': 'USD'}</t>
+          <t>{'rate': 6.596375801676327e-05, 'diff': -4.58, 'diff7d': -8.68, 'ts': 1675485660, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 89199.99991248, 'volDiff1': 6.3761939884296766, 'volDiff7': 21.32794046181195, 'volDiff30': 18.76341203977603, 'diff30d': -89.09726477912302, 'bid': 0.00034117, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O373" t="n">
@@ -28759,7 +28773,7 @@
       </c>
       <c r="G410" t="inlineStr"/>
       <c r="H410" t="n">
-        <v>1674974779</v>
+        <v>1675322609</v>
       </c>
       <c r="I410" t="n">
         <v>1</v>
@@ -29296,7 +29310,7 @@
       </c>
       <c r="F418" t="inlineStr">
         <is>
-          <t>47923911882692106491595726</t>
+          <t>47947781016974204097575726</t>
         </is>
       </c>
       <c r="G418" t="inlineStr">
@@ -29305,13 +29319,13 @@
         </is>
       </c>
       <c r="H418" t="n">
-        <v>1674973528</v>
+        <v>1675442328</v>
       </c>
       <c r="I418" t="n">
-        <v>37398</v>
+        <v>37401</v>
       </c>
       <c r="J418" t="n">
-        <v>2586</v>
+        <v>2588</v>
       </c>
       <c r="K418" t="inlineStr"/>
       <c r="L418" t="inlineStr"/>
@@ -29369,7 +29383,7 @@
       </c>
       <c r="G419" t="inlineStr"/>
       <c r="H419" t="n">
-        <v>1674967036</v>
+        <v>1675130517</v>
       </c>
       <c r="I419" t="n">
         <v>21</v>
@@ -29437,13 +29451,13 @@
         </is>
       </c>
       <c r="H420" t="n">
-        <v>1675053663</v>
+        <v>1675485899</v>
       </c>
       <c r="I420" t="n">
         <v>2</v>
       </c>
       <c r="J420" t="n">
-        <v>1402</v>
+        <v>1747</v>
       </c>
       <c r="K420" t="inlineStr">
         <is>
@@ -29455,12 +29469,10 @@
           <t>/images/VITA81f8f0bb.png</t>
         </is>
       </c>
-      <c r="M420" t="n">
-        <v>0</v>
-      </c>
+      <c r="M420" t="inlineStr"/>
       <c r="N420" t="inlineStr">
         <is>
-          <t>{'rate': 1.1253338033622102, 'diff': 3.6, 'diff7d': 0.47, 'ts': 1675055460, 'marketCapUsd': 26433785.56389664, 'availableSupply': 0, 'volume24h': 27375.49512018, 'volDiff1': 6.2949674183574444, 'volDiff7': 126.22281828157534, 'bid': 1.99, 'volDiff30': 199.1487788357428, 'currency': 'USD'}</t>
+          <t>{'rate': 1.5478657325348504, 'diff': 0.81, 'diff7d': 44.42, 'ts': 1675485660, 'marketCapUsd': 36354029.771593906, 'availableSupply': 0, 'volume24h': 97924.89048979, 'volDiff1': -43.87456629283798, 'volDiff7': 3228.096686199122, 'bid': 1.99, 'volDiff30': 3704.3014347287494, 'diff30d': 93.7592946301317, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O420" t="n">
@@ -29506,18 +29518,18 @@
       </c>
       <c r="F421" t="inlineStr">
         <is>
-          <t>2892558503043067940458519</t>
+          <t>2863602827788996538648418</t>
         </is>
       </c>
       <c r="G421" t="inlineStr"/>
       <c r="H421" t="n">
-        <v>1675036503</v>
+        <v>1675480215</v>
       </c>
       <c r="I421" t="n">
-        <v>13227</v>
+        <v>13238</v>
       </c>
       <c r="J421" t="n">
-        <v>3210</v>
+        <v>3218</v>
       </c>
       <c r="K421" t="inlineStr">
         <is>
@@ -29534,7 +29546,7 @@
       </c>
       <c r="N421" t="inlineStr">
         <is>
-          <t>{'rate': 2.7729125337191496, 'diff': -0.1, 'diff7d': -0.26, 'ts': 1675055460, 'marketCapUsd': 8020811.72760403, 'availableSupply': 2892558.50304307, 'volume24h': 370271.4373458, 'volDiff1': 17.87877826384188, 'volDiff7': -40.87880677693517, 'volDiff30': 80.37212496668613, 'diff30d': -1.8491904135416917, 'bid': 3.02, 'currency': 'USD'}</t>
+          <t>{'rate': 2.7686163875389806, 'diff': -0.17, 'diff7d': -0.33, 'ts': 1675485660, 'marketCapUsd': 7928217.716419591, 'availableSupply': 2863602.827789, 'volume24h': 310216.22037521, 'volDiff1': 2.9030210591934207, 'volDiff7': -67.6281248634539, 'volDiff30': 100.51292262521278, 'diff30d': -1.8491904135416917, 'bid': 3.02, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O421" t="n">
@@ -29584,7 +29596,7 @@
       </c>
       <c r="F422" t="inlineStr">
         <is>
-          <t>293767517732247847839741193260</t>
+          <t>292004636293749183839741193260</t>
         </is>
       </c>
       <c r="G422" t="inlineStr">
@@ -29593,13 +29605,13 @@
         </is>
       </c>
       <c r="H422" t="n">
-        <v>1675055125</v>
+        <v>1675485534</v>
       </c>
       <c r="I422" t="n">
-        <v>60866</v>
+        <v>61025</v>
       </c>
       <c r="J422" t="n">
-        <v>79448</v>
+        <v>79767</v>
       </c>
       <c r="K422" t="inlineStr">
         <is>
@@ -29616,7 +29628,7 @@
       </c>
       <c r="N422" t="inlineStr">
         <is>
-          <t>{'rate': 0.0001699855894316103, 'diff': 0.57, 'diff7d': -4.05, 'ts': 1675055460, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 121723.96200683671, 'volDiff1': -1.5366867893310285, 'volDiff7': 9.812087711198416, 'volDiff30': -13.97640295506524, 'diff30d': -31.00100328911269, 'bid': 86.38, 'currency': 'USD'}</t>
+          <t>{'rate': 0.00019741977350819334, 'diff': 12.07, 'diff7d': 15.63, 'ts': 1675485660, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 531466.9253597641, 'volDiff1': 460.0053190923411, 'volDiff7': 132.2725590184261, 'volDiff30': 14.796496663541618, 'diff30d': -31.00100328911269, 'bid': 86.38, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O422" t="n">
@@ -29671,7 +29683,7 @@
         </is>
       </c>
       <c r="H423" t="n">
-        <v>1674865657</v>
+        <v>1675324205</v>
       </c>
       <c r="I423" t="n">
         <v>0</v>
@@ -29694,7 +29706,7 @@
       </c>
       <c r="N423" t="inlineStr">
         <is>
-          <t>{'rate': 8.997047905365154e-08, 'diff': 0, 'diff7d': -27.43, 'ts': 1675054200, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 0, 'volDiff1': -100, 'volDiff7': -53.095048061048814, 'volDiff30': -80.20411181981981, 'currency': 'USD'}</t>
+          <t>{'rate': 8.997047905365154e-08, 'diff': 0, 'diff7d': -1.6, 'ts': 1675482600, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 0, 'volDiff1': -100, 'volDiff7': -100, 'volDiff30': -32.32219076451716, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O423" t="n">
@@ -29749,7 +29761,7 @@
         </is>
       </c>
       <c r="H424" t="n">
-        <v>1674949056</v>
+        <v>1675480813</v>
       </c>
       <c r="I424" t="n">
         <v>1</v>
@@ -29772,7 +29784,7 @@
       </c>
       <c r="N424" t="inlineStr">
         <is>
-          <t>{'rate': 0.004568799719913078, 'diff': 2.63, 'diff7d': 7.59, 'ts': 1675054200, 'marketCapUsd': 1736402.8862997831, 'availableSupply': 0, 'volume24h': 20197.135426240242, 'volDiff1': 19520.087196186327, 'volDiff7': -33.2627655938164, 'volDiff30': 23.972637008264442, 'bid': 0.01047956, 'diff30d': 81.73456707845614, 'currency': 'USD'}</t>
+          <t>{'rate': 0.004404440930907627, 'diff': 0.86, 'diff7d': 7.69, 'ts': 1675482600, 'marketCapUsd': 1768933.8992274764, 'availableSupply': 0, 'volume24h': 19390.041066059774, 'volDiff1': 137161.3966851338, 'volDiff7': -63.914386352585666, 'volDiff30': 56.74636412091661, 'bid': 0.01047956, 'diff30d': 81.73456707845614, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O424" t="n">
@@ -29827,13 +29839,13 @@
       </c>
       <c r="G425" t="inlineStr"/>
       <c r="H425" t="n">
-        <v>1675027079</v>
+        <v>1675482121</v>
       </c>
       <c r="I425" t="n">
         <v>1</v>
       </c>
       <c r="J425" t="n">
-        <v>1121</v>
+        <v>1127</v>
       </c>
       <c r="K425" t="inlineStr">
         <is>
@@ -29850,7 +29862,7 @@
       </c>
       <c r="N425" t="inlineStr">
         <is>
-          <t>{'rate': 64.74838876068483, 'diff': 1.34, 'diff7d': -0.31, 'ts': 1675055460, 'marketCapUsd': 324385.96082232555, 'availableSupply': 0, 'volume24h': 79372.9748561834, 'volDiff1': 40.650406911534475, 'volDiff7': 22.96709171241676, 'volDiff30': 65.47270613732655, 'bid': 352.62, 'currency': 'USD'}</t>
+          <t>{'rate': 80.53074384270387, 'diff': 7.33, 'diff7d': 25.61, 'ts': 1675485660, 'marketCapUsd': 337613.41296254855, 'availableSupply': 0, 'volume24h': 79821.16841808209, 'volDiff1': 22.017270319199127, 'volDiff7': 9.639808547652962, 'volDiff30': 213.11511557959835, 'bid': 352.62, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O425" t="n">
@@ -29909,13 +29921,13 @@
         </is>
       </c>
       <c r="H426" t="n">
-        <v>1675055007</v>
+        <v>1675485425</v>
       </c>
       <c r="I426" t="n">
         <v>1</v>
       </c>
       <c r="J426" t="n">
-        <v>106711</v>
+        <v>107139</v>
       </c>
       <c r="K426" t="inlineStr">
         <is>
@@ -29927,10 +29939,12 @@
           <t>/images/1INCH11111111.png</t>
         </is>
       </c>
-      <c r="M426" t="inlineStr"/>
+      <c r="M426" t="n">
+        <v>0</v>
+      </c>
       <c r="N426" t="inlineStr">
         <is>
-          <t>{'rate': 0.5306562648754538, 'diff': 0.37, 'diff7d': -0.21, 'ts': 1675055760, 'marketCapUsd': 423101505.7419307, 'availableSupply': 797317460.9391139, 'volume24h': 30305534.1091767, 'volDiff1': -7.675725339768817, 'volDiff7': 16.252352294241646, 'volDiff30': 122.03727485586259, 'diff30d': 38.39776804953544, 'bid': 1.27, 'currency': 'USD'}</t>
+          <t>{'rate': 0.5580927151166946, 'diff': 1.52, 'diff7d': 2.54, 'ts': 1675485960, 'marketCapUsd': 441713066.1288767, 'availableSupply': 791468969.5179349, 'volume24h': 43584561.95482036, 'volDiff1': -22.290626031159093, 'volDiff7': -24.95759882716419, 'volDiff30': 185.17501345771865, 'diff30d': 41.87313255487743, 'bid': 1.27, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O426" t="n">
@@ -30385,13 +30399,13 @@
         </is>
       </c>
       <c r="H433" t="n">
-        <v>1675055554</v>
+        <v>1675485700</v>
       </c>
       <c r="I433" t="n">
         <v>2606</v>
       </c>
       <c r="J433" t="n">
-        <v>11665</v>
+        <v>11686</v>
       </c>
       <c r="K433" t="inlineStr">
         <is>
@@ -30406,7 +30420,7 @@
       <c r="M433" t="inlineStr"/>
       <c r="N433" t="inlineStr">
         <is>
-          <t>{'rate': 0.004031848735075609, 'diff': 0.58, 'diff7d': -4.19, 'ts': 1675055460, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 240612.39023758, 'volDiff1': -13.204539362410728, 'volDiff7': -9.578521654392048, 'volDiff30': -36.84401255801236, 'diff30d': -8.483000057035653, 'bid': 0.03932069, 'currency': 'USD'}</t>
+          <t>{'rate': 0.00521027945702685, 'diff': -4.54, 'diff7d': 28.56, 'ts': 1675485660, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 261527.14237237, 'volDiff1': -10.670257164557086, 'volDiff7': -0.5352217734903206, 'volDiff30': -33.9304447742186, 'diff30d': -8.483000057035653, 'bid': 0.03932069, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O433" t="n">
@@ -31449,13 +31463,13 @@
         </is>
       </c>
       <c r="H449" t="n">
-        <v>1674744050</v>
+        <v>1675261718</v>
       </c>
       <c r="I449" t="n">
         <v>1</v>
       </c>
       <c r="J449" t="n">
-        <v>3560</v>
+        <v>3557</v>
       </c>
       <c r="K449" t="inlineStr">
         <is>
@@ -31472,7 +31486,7 @@
       </c>
       <c r="N449" t="inlineStr">
         <is>
-          <t>{'rate': 0.6335627020522584, 'diff': 0.16, 'diff7d': 1.94, 'ts': 1675055460, 'marketCapUsd': 19014148.659322992, 'availableSupply': 30011471, 'volume24h': 866400.58547916, 'volDiff1': 7.064559405438558, 'volDiff7': 11.204781248041982, 'volDiff30': 11.60356137026777, 'diff30d': 49.51982671867984, 'bid': 3.19, 'currency': 'USD'}</t>
+          <t>{'rate': 0.6616307488267663, 'diff': -0.34, 'diff7d': 1.06, 'ts': 1675485660, 'marketCapUsd': 19856512.03112278, 'availableSupply': 30011471, 'volume24h': 754639.3060149, 'volDiff1': -5.232335326977662, 'volDiff7': 11.152672962057594, 'volDiff30': -1.1284318153561372, 'diff30d': 49.51982671867984, 'bid': 3.19, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O449" t="n">
@@ -33004,18 +33018,18 @@
       </c>
       <c r="F472" t="inlineStr">
         <is>
-          <t>878586986087773104766000</t>
+          <t>878646228168904453133018</t>
         </is>
       </c>
       <c r="G472" t="inlineStr"/>
       <c r="H472" t="n">
-        <v>1675055228</v>
+        <v>1675485797</v>
       </c>
       <c r="I472" t="n">
-        <v>475026</v>
+        <v>477092</v>
       </c>
       <c r="J472" t="n">
-        <v>18513</v>
+        <v>18443</v>
       </c>
       <c r="K472" t="inlineStr">
         <is>
@@ -33081,13 +33095,13 @@
       </c>
       <c r="G473" t="inlineStr"/>
       <c r="H473" t="n">
-        <v>1675055378</v>
+        <v>1675485526</v>
       </c>
       <c r="I473" t="n">
         <v>0</v>
       </c>
       <c r="J473" t="n">
-        <v>464492</v>
+        <v>464584</v>
       </c>
       <c r="K473" t="inlineStr">
         <is>
@@ -33104,7 +33118,7 @@
       </c>
       <c r="N473" t="inlineStr">
         <is>
-          <t>{'rate': 0.26639979182689916, 'diff': 1.27, 'diff7d': 5.23, 'ts': 1675055760, 'marketCapUsd': 396968002.6293411, 'availableSupply': 1490121294.4163349, 'volume24h': 54481138.73356746, 'volDiff1': 63.69630482015981, 'volDiff7': 10.92195496506649, 'volDiff30': 144.68204220382458, 'diff30d': 60.3289248775975, 'bid': 0.637052, 'currency': 'USD'}</t>
+          <t>{'rate': 0.27465435284433515, 'diff': 2.77, 'diff7d': 1.84, 'ts': 1675485960, 'marketCapUsd': 410022431.4174951, 'availableSupply': 1492867042.4163349, 'volume24h': 36243966.1149591, 'volDiff1': -1.5916842116121188, 'volDiff7': -13.628895900448, 'volDiff30': 175.5345831811211, 'diff30d': 53.333093286198874, 'bid': 0.637052, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O473" t="n">
@@ -33291,13 +33305,13 @@
       </c>
       <c r="G476" t="inlineStr"/>
       <c r="H476" t="n">
-        <v>1675054843</v>
+        <v>1675484995</v>
       </c>
       <c r="I476" t="n">
         <v>1</v>
       </c>
       <c r="J476" t="n">
-        <v>68667</v>
+        <v>68919</v>
       </c>
       <c r="K476" t="inlineStr">
         <is>
@@ -33314,7 +33328,7 @@
       </c>
       <c r="N476" t="inlineStr">
         <is>
-          <t>{'rate': 11.847341953025087, 'diff': 2.38, 'diff7d': -10.41, 'ts': 1675055760, 'marketCapUsd': 1197092408.8047204, 'availableSupply': 101043121.19555697, 'volume24h': 253605935.03707263, 'volDiff1': 7.138963211416737, 'volDiff7': 65.34928051046873, 'volDiff30': 97.65541524352517, 'diff30d': 96.85739467744335, 'bid': 35.73, 'currency': 'USD'}</t>
+          <t>{'rate': 11.321340054615687, 'diff': 1.01, 'diff7d': -5.17, 'ts': 1675485960, 'marketCapUsd': 1141980575.8229473, 'availableSupply': 100869735.41240501, 'volume24h': 110517825.54745996, 'volDiff1': -25.3067736694653, 'volDiff7': -60.190181071205764, 'volDiff30': 199.6756171450109, 'diff30d': 67.24298575209474, 'bid': 35.73, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O476" t="n">
@@ -33645,13 +33659,13 @@
         </is>
       </c>
       <c r="H481" t="n">
-        <v>1672519284</v>
+        <v>1675311269</v>
       </c>
       <c r="I481" t="n">
         <v>1</v>
       </c>
       <c r="J481" t="n">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="K481" t="inlineStr"/>
       <c r="L481" t="inlineStr"/>
@@ -37357,13 +37371,13 @@
       </c>
       <c r="G536" t="inlineStr"/>
       <c r="H536" t="n">
-        <v>1675055213</v>
+        <v>1675485568</v>
       </c>
       <c r="I536" t="n">
         <v>1</v>
       </c>
       <c r="J536" t="n">
-        <v>111407</v>
+        <v>112333</v>
       </c>
       <c r="K536" t="inlineStr">
         <is>
@@ -37380,7 +37394,7 @@
       </c>
       <c r="N536" t="inlineStr">
         <is>
-          <t>{'rate': 6.19616414129678, 'diff': 3.09, 'diff7d': 7.05, 'ts': 1675055760, 'marketCapUsd': 2283867376.45611, 'availableSupply': 368593750, 'volume24h': 156154264.28287467, 'volDiff1': -12.012438173891837, 'volDiff7': 17.65103186011126, 'volDiff30': 67.80494419755877, 'diff30d': 71.3397989796764, 'bid': 22.19, 'currency': 'USD'}</t>
+          <t>{'rate': 5.9508153847279415, 'diff': 0.68, 'diff7d': -4.88, 'ts': 1675485960, 'marketCapUsd': 2193433358.214565, 'availableSupply': 368593750, 'volume24h': 118707981.72523636, 'volDiff1': -23.947078151991136, 'volDiff7': -41.46094497828952, 'volDiff30': 84.02165556144709, 'diff30d': 47.3505716643794, 'bid': 22.19, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O536" t="n">
@@ -37839,13 +37853,13 @@
         </is>
       </c>
       <c r="H543" t="n">
-        <v>1675049329</v>
+        <v>1675472987</v>
       </c>
       <c r="I543" t="n">
         <v>2257</v>
       </c>
       <c r="J543" t="n">
-        <v>5916</v>
+        <v>5917</v>
       </c>
       <c r="K543" t="inlineStr">
         <is>
@@ -37862,7 +37876,7 @@
       </c>
       <c r="N543" t="inlineStr">
         <is>
-          <t>{'rate': 1.7284543745828063e-08, 'diff': 1.64, 'diff7d': -15.62, 'ts': 1675055460, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 228598.19823568608, 'volDiff1': 60.995375435176584, 'volDiff7': -90.29612533724536, 'volDiff30': 23.411737843491125, 'diff30d': 15.530630051549267, 'currency': 'USD'}</t>
+          <t>{'rate': 1.8542791857015716e-08, 'diff': 10.56, 'diff7d': 7.11, 'ts': 1675485660, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 265676.46239047946, 'volDiff1': 90.08295948862332, 'volDiff7': -83.84987443430997, 'volDiff30': 19.59110464082589, 'diff30d': 15.530630051549267, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O543" t="n">
@@ -37983,7 +37997,7 @@
         </is>
       </c>
       <c r="H545" t="n">
-        <v>1675017241</v>
+        <v>1675424875</v>
       </c>
       <c r="I545" t="n">
         <v>1</v>
@@ -38006,7 +38020,7 @@
       </c>
       <c r="N545" t="inlineStr">
         <is>
-          <t>{'rate': 0.007822215389023206, 'diff': 3.16, 'diff7d': 8.26, 'ts': 1675054200, 'marketCapUsd': 322040.45887871285, 'availableSupply': 0, 'volume24h': 22.837575342936233, 'volDiff1': -97.1750722298277, 'volDiff7': 601.6091212069933, 'volDiff30': 117.37552962031936, 'currency': 'USD'}</t>
+          <t>{'rate': 0.008931622843992465, 'diff': 2.63, 'diff7d': 26.73, 'ts': 1675482600, 'marketCapUsd': 369960.9208678252, 'availableSupply': 0, 'volume24h': 195.47320071826815, 'volDiff1': -71.58392965247666, 'volDiff7': -40.52907188507133, 'volDiff30': 91.39012621223384, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O545" t="n">
@@ -38331,7 +38345,7 @@
       </c>
       <c r="G550" t="inlineStr"/>
       <c r="H550" t="n">
-        <v>1674866602</v>
+        <v>1675355074</v>
       </c>
       <c r="I550" t="n">
         <v>1</v>
@@ -38399,7 +38413,7 @@
         </is>
       </c>
       <c r="H551" t="n">
-        <v>1675020196</v>
+        <v>1675353663</v>
       </c>
       <c r="I551" t="n">
         <v>54961</v>
@@ -38422,7 +38436,7 @@
       </c>
       <c r="N551" t="inlineStr">
         <is>
-          <t>{'rate': 0.07101610994685453, 'diff': 1.26, 'diff7d': -2.2, 'ts': 1675055460, 'marketCapUsd': 686638.6844908247, 'availableSupply': 0, 'volume24h': 68046.81844951, 'volDiff1': 1.839939072005123, 'volDiff7': 6.601228802434321, 'volDiff30': -25.31366919145718, 'diff30d': 99.85961621149474, 'bid': 0.166991, 'currency': 'USD'}</t>
+          <t>{'rate': 0.07785052188870818, 'diff': -0.19, 'diff7d': 10.25, 'ts': 1675485660, 'marketCapUsd': 785233.0611026685, 'availableSupply': 0, 'volume24h': 65292.59298352, 'volDiff1': -18.631928378699584, 'volDiff7': 67.24849620365515, 'volDiff30': -20.7053931105539, 'diff30d': 99.85961621149474, 'bid': 0.166991, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O551" t="n">
@@ -38477,13 +38491,13 @@
         </is>
       </c>
       <c r="H552" t="n">
-        <v>1675026945</v>
+        <v>1675241881</v>
       </c>
       <c r="I552" t="n">
         <v>4</v>
       </c>
       <c r="J552" t="n">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="K552" t="inlineStr">
         <is>
@@ -38500,7 +38514,7 @@
       </c>
       <c r="N552" t="inlineStr">
         <is>
-          <t>{'rate': 0.01721618640863107, 'diff': -3.79, 'diff7d': 5.28, 'ts': 1675054200, 'marketCapUsd': 1226832.9258199458, 'availableSupply': 71260434.61082019, 'volume24h': 184.0639482067499, 'volDiff1': -97.10029887792467, 'volDiff7': 446.2982558446571, 'volDiff30': 92.43455782974931, 'bid': 0.139814, 'currency': 'USD'}</t>
+          <t>{'rate': 0.017592850180180284, 'diff': 2.06, 'diff7d': -3.04, 'ts': 1675482600, 'marketCapUsd': 1253674.1498826933, 'availableSupply': 71260434.61082019, 'volume24h': 67.89311112, 'volDiff1': 1.8091239428172088, 'volDiff7': -21.989111189370902, 'volDiff30': 73.25970578584531, 'bid': 0.139814, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O552" t="n">
@@ -38555,13 +38569,13 @@
         </is>
       </c>
       <c r="H553" t="n">
-        <v>1673461073</v>
+        <v>1675361990</v>
       </c>
       <c r="I553" t="n">
         <v>1</v>
       </c>
       <c r="J553" t="n">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="K553" t="inlineStr">
         <is>
@@ -38582,7 +38596,7 @@
         </is>
       </c>
       <c r="O553" t="n">
-        <v>5.900168059745151e+16</v>
+        <v>5.900195921187062e+16</v>
       </c>
       <c r="P553" t="n">
         <v>0</v>
@@ -38592,7 +38606,7 @@
       </c>
       <c r="R553" t="inlineStr">
         <is>
-          <t>59001680597451515</t>
+          <t>59001959211870614</t>
         </is>
       </c>
       <c r="S553" t="inlineStr"/>
@@ -38711,7 +38725,9 @@
       </c>
       <c r="K555" t="inlineStr"/>
       <c r="L555" t="inlineStr"/>
-      <c r="M555" t="inlineStr"/>
+      <c r="M555" t="n">
+        <v>0</v>
+      </c>
       <c r="N555" t="b">
         <v>0</v>
       </c>
@@ -38792,7 +38808,7 @@
         <v>0</v>
       </c>
       <c r="O556" t="n">
-        <v>5.716591671097215e+22</v>
+        <v>5.716606845035414e+22</v>
       </c>
       <c r="P556" t="n">
         <v>0</v>
@@ -38802,7 +38818,7 @@
       </c>
       <c r="R556" t="inlineStr">
         <is>
-          <t>57165916710972150375497</t>
+          <t>57166068450354148488328</t>
         </is>
       </c>
       <c r="S556" t="inlineStr"/>
@@ -38998,7 +39014,7 @@
       </c>
       <c r="N559" t="inlineStr">
         <is>
-          <t>{'rate': 0.00038491961675635574, 'diff': 2.38, 'diff7d': 3.42, 'ts': 1675054200, 'marketCapUsd': 338112.88518948684, 'availableSupply': 878398685, 'volume24h': 0.1872415102610319, 'volDiff1': -100, 'volDiff7': -100, 'volDiff30': -100, 'bid': 3.105e-05, 'currency': 'USD'}</t>
+          <t>{'rate': 0.0004022510246775007, 'diff': 2.7, 'diff7d': 7.03, 'ts': 1675482600, 'marketCapUsd': 353336.7711166192, 'availableSupply': 878398685, 'volume24h': 0, 'volDiff1': -100, 'volDiff7': -100, 'volDiff30': -100, 'bid': 3.105e-05, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O559" t="n">
@@ -40063,18 +40079,18 @@
       </c>
       <c r="F575" t="inlineStr">
         <is>
-          <t>703275800000000000000000</t>
+          <t>703367560000000000000000</t>
         </is>
       </c>
       <c r="G575" t="inlineStr"/>
       <c r="H575" t="n">
-        <v>1675050399</v>
+        <v>1675483270</v>
       </c>
       <c r="I575" t="n">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="J575" t="n">
-        <v>14447</v>
+        <v>14458</v>
       </c>
       <c r="K575" t="inlineStr">
         <is>
@@ -40091,7 +40107,7 @@
       </c>
       <c r="N575" t="inlineStr">
         <is>
-          <t>{'rate': 39.56721562638073, 'diff': 0.82, 'diff7d': 7.59, 'ts': 1675055760, 'marketCapUsd': 26952190.456471488, 'availableSupply': 681174.806713, 'volume24h': 3436972.18087859, 'volDiff1': 16.25488422655144, 'volDiff7': 88.79604631255688, 'volDiff30': 14.207485417987598, 'diff30d': 36.16826827140042, 'bid': 87.09, 'currency': 'USD'}</t>
+          <t>{'rate': 38.275951115494806, 'diff': 1.49, 'diff7d': -0.51, 'ts': 1675485960, 'marketCapUsd': 26072613.602853414, 'availableSupply': 681174.806713, 'volume24h': 1515523.14746765, 'volDiff1': -16.54189199988177, 'volDiff7': 35.17659470204043, 'volDiff30': 84.71601613275342, 'diff30d': 27.645070774980994, 'bid': 87.09, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O575" t="n">
@@ -40150,13 +40166,13 @@
         </is>
       </c>
       <c r="H576" t="n">
-        <v>1675031528</v>
+        <v>1675304062</v>
       </c>
       <c r="I576" t="n">
         <v>1281</v>
       </c>
       <c r="J576" t="n">
-        <v>5497</v>
+        <v>5496</v>
       </c>
       <c r="K576" t="inlineStr">
         <is>
@@ -40173,7 +40189,7 @@
       </c>
       <c r="N576" t="inlineStr">
         <is>
-          <t>{'rate': 5.70163902932738e-10, 'diff': -0.33, 'diff7d': -10.93, 'ts': 1675054200, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 1785.8897596680922, 'volDiff1': 43.141179553908074, 'volDiff7': -33.470974434357586, 'volDiff30': 197.26866741998634, 'currency': 'USD'}</t>
+          <t>{'rate': 5.89871056029321e-10, 'diff': 3.69, 'diff7d': -4.85, 'ts': 1675482600, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 6015.684665971153, 'volDiff1': 96.94488078430092, 'volDiff7': -31.073404686173944, 'volDiff30': 318.6843035015599, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O576" t="n">
@@ -40494,13 +40510,13 @@
         </is>
       </c>
       <c r="H581" t="n">
-        <v>1675033793</v>
+        <v>1675482686</v>
       </c>
       <c r="I581" t="n">
         <v>1</v>
       </c>
       <c r="J581" t="n">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="K581" t="inlineStr">
         <is>
@@ -40517,7 +40533,7 @@
       </c>
       <c r="N581" t="inlineStr">
         <is>
-          <t>{'rate': 0.020283303724734553, 'diff': 1.66, 'diff7d': 5.36, 'ts': 1675054200, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 244.47428617996337, 'volDiff1': -74.30507360275769, 'volDiff7': -57.450097830743616, 'volDiff30': -38.64374606672306, 'currency': 'USD'}</t>
+          <t>{'rate': 0.016134356851813792, 'diff': -17.5, 'diff7d': -18.42, 'ts': 1675482600, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 2591.256366377672, 'volDiff1': 598.3891024286243, 'volDiff7': 31.002423817350518, 'volDiff30': -55.88759200512969, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O581" t="n">
@@ -40770,13 +40786,13 @@
       </c>
       <c r="G585" t="inlineStr"/>
       <c r="H585" t="n">
-        <v>1675049033</v>
+        <v>1675479920</v>
       </c>
       <c r="I585" t="n">
         <v>1</v>
       </c>
       <c r="J585" t="n">
-        <v>1671</v>
+        <v>1663</v>
       </c>
       <c r="K585" t="inlineStr">
         <is>
@@ -40793,7 +40809,7 @@
       </c>
       <c r="N585" t="inlineStr">
         <is>
-          <t>{'rate': 0.006198717836684211, 'diff': -1.9, 'diff7d': -3.22, 'ts': 1675055460, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 78551.8804583, 'volDiff1': -16.140285650685698, 'volDiff7': 40.899563315222196, 'volDiff30': 10.431852796905034, 'bid': 0.01559595, 'currency': 'USD'}</t>
+          <t>{'rate': 0.00306033682694983, 'diff': -6.48, 'diff7d': -51.47, 'ts': 1675485660, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 237228.6857774, 'volDiff1': -4.449717228859569, 'volDiff7': 95.16650279080886, 'volDiff30': 121.59109319865581, 'bid': 0.01559595, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O585" t="n">
@@ -40844,13 +40860,13 @@
       </c>
       <c r="G586" t="inlineStr"/>
       <c r="H586" t="n">
-        <v>1675047345</v>
+        <v>1675438535</v>
       </c>
       <c r="I586" t="n">
         <v>101091</v>
       </c>
       <c r="J586" t="n">
-        <v>10157</v>
+        <v>10151</v>
       </c>
       <c r="K586" t="inlineStr">
         <is>
@@ -40867,7 +40883,7 @@
       </c>
       <c r="N586" t="inlineStr">
         <is>
-          <t>{'rate': 1.5772534266141427e-08, 'diff': 33.97, 'diff7d': 3.78, 'ts': 1675054200, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 3915.98108576148, 'volDiff1': 187.07667169987332, 'volDiff7': -64.74896532246815, 'volDiff30': 265.2999312536765, 'diff30d': -1.2613022227294977, 'bid': 7.9262e-08, 'currency': 'USD'}</t>
+          <t>{'rate': 1.1684597347962378e-08, 'diff': -9.04, 'diff7d': -11.14, 'ts': 1675482600, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 2232.3517803481877, 'volDiff1': -13.503513481696132, 'volDiff7': 489.2675749440773, 'volDiff30': 607.8510626634151, 'diff30d': -1.2613022227294977, 'bid': 7.9262e-08, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O586" t="n">
@@ -40918,13 +40934,13 @@
       </c>
       <c r="G587" t="inlineStr"/>
       <c r="H587" t="n">
-        <v>1675041803</v>
+        <v>1675467891</v>
       </c>
       <c r="I587" t="n">
         <v>1</v>
       </c>
       <c r="J587" t="n">
-        <v>2790</v>
+        <v>2802</v>
       </c>
       <c r="K587" t="inlineStr">
         <is>
@@ -40941,7 +40957,7 @@
       </c>
       <c r="N587" t="inlineStr">
         <is>
-          <t>{'rate': 0.17327956395891175, 'diff': 1.97, 'diff7d': 1.91, 'ts': 1675055460, 'marketCapUsd': 11382792.250911532, 'availableSupply': 65690332.95588528, 'volume24h': 128303.24940528, 'volDiff1': -9.933788704938479, 'volDiff7': -3.3865630347475673, 'volDiff30': 2.9213165010749407, 'diff30d': -42.40592351350874, 'bid': 0.700189, 'currency': 'USD'}</t>
+          <t>{'rate': 0.2118632359652842, 'diff': 12.19, 'diff7d': 27.18, 'ts': 1675485660, 'marketCapUsd': 14026821.473546308, 'availableSupply': 66206963.23096252, 'volume24h': 206697.16156224, 'volDiff1': 17.389150116240984, 'volDiff7': 9.724022640436687, 'volDiff30': 1.2506863546953184, 'diff30d': -42.40592351350874, 'bid': 0.700189, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O587" t="n">
@@ -40996,13 +41012,13 @@
         </is>
       </c>
       <c r="H588" t="n">
-        <v>1674616659</v>
+        <v>1675326196</v>
       </c>
       <c r="I588" t="n">
         <v>6</v>
       </c>
       <c r="J588" t="n">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="K588" t="inlineStr"/>
       <c r="L588" t="inlineStr"/>
@@ -41128,13 +41144,13 @@
         </is>
       </c>
       <c r="H590" t="n">
-        <v>1674955742</v>
+        <v>1675478178</v>
       </c>
       <c r="I590" t="n">
         <v>1</v>
       </c>
       <c r="J590" t="n">
-        <v>1679</v>
+        <v>1682</v>
       </c>
       <c r="K590" t="inlineStr">
         <is>
@@ -41151,11 +41167,11 @@
       </c>
       <c r="N590" t="inlineStr">
         <is>
-          <t>{'rate': 0.0009555983343927552, 'diff': 2.61, 'diff7d': 9.22, 'ts': 1675054200, 'marketCapUsd': 801610.4235111224, 'availableSupply': 838857074.84046, 'volume24h': 845.6115542457087, 'volDiff1': -88.62538173273497, 'volDiff7': 418.9626223389687, 'volDiff30': 107.86026496351258, 'bid': 0.00338377, 'currency': 'USD'}</t>
+          <t>{'rate': 0.0009658829238995152, 'diff': 3.3, 'diff7d': 3.26, 'ts': 1675482600, 'marketCapUsd': 810235.9415905538, 'availableSupply': 838855229.2853725, 'volume24h': 1883.614626696616, 'volDiff1': 81.3271770480444, 'volDiff7': 202.90215961318336, 'volDiff30': 86.23509788292421, 'bid': 0.00338377, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O590" t="n">
-        <v>283831446187625</v>
+        <v>283865514938806</v>
       </c>
       <c r="P590" t="n">
         <v>0</v>
@@ -41165,7 +41181,7 @@
       </c>
       <c r="R590" t="inlineStr">
         <is>
-          <t>283831446187625</t>
+          <t>283865514938806</t>
         </is>
       </c>
       <c r="S590" t="inlineStr"/>
@@ -41270,13 +41286,13 @@
         </is>
       </c>
       <c r="H592" t="n">
-        <v>1675054607</v>
+        <v>1675485284</v>
       </c>
       <c r="I592" t="n">
         <v>8</v>
       </c>
       <c r="J592" t="n">
-        <v>14032</v>
+        <v>14353</v>
       </c>
       <c r="K592" t="inlineStr">
         <is>
@@ -41293,7 +41309,7 @@
       </c>
       <c r="N592" t="inlineStr">
         <is>
-          <t>{'rate': 0.01672710156511399, 'diff': 0.71, 'diff7d': 13.66, 'ts': 1675055760, 'marketCapUsd': 20606300.686825648, 'availableSupply': 1231911016.18, 'volume24h': 1172882.27510888, 'volDiff1': 27.50395221580189, 'volDiff7': -50.007307412200305, 'volDiff30': 135320.87626852293, 'bid': 0.0007753, 'diff30d': 6427.19502116074, 'currency': 'USD'}</t>
+          <t>{'rate': 0.01660613940974979, 'diff': -4.12, 'diff7d': 2.51, 'ts': 1675485960, 'marketCapUsd': 20457286.075091608, 'availableSupply': 1231911016.18, 'volume24h': 1289227.29659874, 'volDiff1': -11.052621302874599, 'volDiff7': -28.862862448987855, 'volDiff30': 35433.27596673799, 'bid': 0.0007753, 'diff30d': 5005.68054583697, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O592" t="n">
@@ -41548,13 +41564,13 @@
         </is>
       </c>
       <c r="H596" t="n">
-        <v>1675045435</v>
+        <v>1675483217</v>
       </c>
       <c r="I596" t="n">
         <v>1</v>
       </c>
       <c r="J596" t="n">
-        <v>19200</v>
+        <v>19218</v>
       </c>
       <c r="K596" t="inlineStr">
         <is>
@@ -41571,11 +41587,11 @@
       </c>
       <c r="N596" t="inlineStr">
         <is>
-          <t>{'rate': 1.711088385156224e-09, 'diff': -66.17, 'diff7d': 17.35, 'ts': 1675055460, 'marketCapUsd': 2098695.5915048826, 'availableSupply': 0, 'volume24h': 12830.47190864, 'volDiff1': -46.969487352080996, 'volDiff7': -54.95967970843811, 'volDiff30': 40.65588576663842, 'diff30d': -86.36420500921457, 'bid': 1.6156e-08, 'currency': 'USD'}</t>
+          <t>{'rate': 2.139799147954091e-09, 'diff': 11.8, 'diff7d': -57.82, 'ts': 1675485660, 'marketCapUsd': 2037937.1628509918, 'availableSupply': 0, 'volume24h': 28159.02776831, 'volDiff1': 165.5936543211243, 'volDiff7': -26.648021022471596, 'volDiff30': 74.86330473233446, 'diff30d': -86.36420500921457, 'bid': 1.6156e-08, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O596" t="n">
-        <v>4.411707376344486e+17</v>
+        <v>4.411904753523486e+17</v>
       </c>
       <c r="P596" t="n">
         <v>0</v>
@@ -41585,7 +41601,7 @@
       </c>
       <c r="R596" t="inlineStr">
         <is>
-          <t>441170737634448570</t>
+          <t>441190475352348625</t>
         </is>
       </c>
       <c r="S596" t="inlineStr"/>
@@ -41617,7 +41633,7 @@
       </c>
       <c r="F597" t="inlineStr">
         <is>
-          <t>336926161831576340655983081</t>
+          <t>336924379719576340655983081</t>
         </is>
       </c>
       <c r="G597" t="inlineStr">
@@ -41626,13 +41642,13 @@
         </is>
       </c>
       <c r="H597" t="n">
-        <v>1675040183</v>
+        <v>1675356804</v>
       </c>
       <c r="I597" t="n">
-        <v>2643</v>
+        <v>2644</v>
       </c>
       <c r="J597" t="n">
-        <v>2103</v>
+        <v>2105</v>
       </c>
       <c r="K597" t="inlineStr"/>
       <c r="L597" t="inlineStr"/>
@@ -41641,7 +41657,7 @@
       </c>
       <c r="N597" t="inlineStr">
         <is>
-          <t>{'rate': 0.0156484230101689, 'diff': 2.81, 'diff7d': 5.07, 'ts': 1675055460, 'marketCapUsd': 1840917.6181889146, 'availableSupply': 117642373.1, 'volume24h': 18961.75986189907, 'volDiff1': 28.85659947737838, 'volDiff7': -46.4897739838368, 'volDiff30': 73.61372390248397, 'diff30d': -24.581922073866608, 'bid': 0.0272723, 'currency': 'USD'}</t>
+          <t>{'rate': 0.014493401738485519, 'diff': -3.08, 'diff7d': -4.1, 'ts': 1675485660, 'marketCapUsd': 1705038.174807102, 'availableSupply': 117642373.1, 'volume24h': 17147.559981119735, 'volDiff1': -2.005057391334063, 'volDiff7': 5.335262910135754, 'volDiff30': 76.05628176393401, 'diff30d': -24.581922073866608, 'bid': 0.0272723, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O597" t="n">
@@ -41696,13 +41712,13 @@
         </is>
       </c>
       <c r="H598" t="n">
-        <v>1675055700</v>
+        <v>1675485053</v>
       </c>
       <c r="I598" t="n">
         <v>0</v>
       </c>
       <c r="J598" t="n">
-        <v>137119</v>
+        <v>135857</v>
       </c>
       <c r="K598" t="inlineStr">
         <is>
@@ -41719,7 +41735,7 @@
       </c>
       <c r="N598" t="inlineStr">
         <is>
-          <t>{'rate': 0.00218654062621433, 'diff': -0.03, 'diff7d': 6.67, 'ts': 1675055760, 'marketCapUsd': 379021455.19693017, 'availableSupply': 173342974126.73712, 'volume24h': 18209891.63149868, 'volDiff1': -26.803425927189906, 'volDiff7': 21.051091703264063, 'volDiff30': 56.32630714475971, 'diff30d': 52.961748175825164, 'bid': 0.00423997, 'currency': 'USD'}</t>
+          <t>{'rate': 0.0021947393113997634, 'diff': 0.56, 'diff7d': -1.52, 'ts': 1675485960, 'marketCapUsd': 380442639.670902, 'availableSupply': 173342974126.73712, 'volume24h': 23094558.95792078, 'volDiff1': 7.121821486193397, 'volDiff7': -20.810696491848873, 'volDiff30': 77.19215985661123, 'diff30d': 49.3660639640693, 'bid': 0.00423997, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O598" t="n">
@@ -41773,7 +41789,7 @@
       </c>
       <c r="F599" t="inlineStr">
         <is>
-          <t>2193227227320146244857883456</t>
+          <t>2193225127320146244857883456</t>
         </is>
       </c>
       <c r="G599" t="inlineStr">
@@ -41782,13 +41798,13 @@
         </is>
       </c>
       <c r="H599" t="n">
-        <v>1675054734</v>
+        <v>1675485301</v>
       </c>
       <c r="I599" t="n">
-        <v>38559</v>
+        <v>38580</v>
       </c>
       <c r="J599" t="n">
-        <v>308688</v>
+        <v>309071</v>
       </c>
       <c r="K599" t="inlineStr">
         <is>
@@ -41805,7 +41821,7 @@
       </c>
       <c r="N599" t="inlineStr">
         <is>
-          <t>{'rate': 0.797515359339395, 'diff': 12.82, 'diff7d': 9.2, 'ts': 1675055760, 'marketCapUsd': 1479458135.812638, 'availableSupply': 1855084191.7804768, 'volume24h': 631915285.2339723, 'volDiff1': 84.5491020545513, 'volDiff7': -24.337974127417525, 'volDiff30': 530.862074944158, 'diff30d': 170.2604239950141, 'bid': 1.74, 'currency': 'USD'}</t>
+          <t>{'rate': 0.7772347785832739, 'diff': -0.41, 'diff7d': 7.5, 'ts': 1675485960, 'marketCapUsd': 1441835951.0518305, 'availableSupply': 1855084191.7804768, 'volume24h': 171467317.50786528, 'volDiff1': -26.755124345303457, 'volDiff7': 24.59274442146797, 'volDiff30': 654.5993139400575, 'diff30d': 139.63065074793434, 'bid': 1.74, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O599" t="n">
@@ -41868,13 +41884,13 @@
         </is>
       </c>
       <c r="H600" t="n">
-        <v>1675054926</v>
+        <v>1675483924</v>
       </c>
       <c r="I600" t="n">
         <v>3</v>
       </c>
       <c r="J600" t="n">
-        <v>203342</v>
+        <v>203651</v>
       </c>
       <c r="K600" t="inlineStr">
         <is>
@@ -41891,7 +41907,7 @@
       </c>
       <c r="N600" t="inlineStr">
         <is>
-          <t>{'rate': 0.46141459994166956, 'diff': 0.99, 'diff7d': 5.18, 'ts': 1675055760, 'marketCapUsd': 461414599.9416696, 'availableSupply': 1000000000, 'volume24h': 48607400.29421297, 'volDiff1': -72.25648394466356, 'volDiff7': -39.52369290144646, 'volDiff30': 297.3679734952517, 'diff30d': 92.10404619421155, 'bid': 1.25, 'currency': 'USD'}</t>
+          <t>{'rate': 0.46547306669395283, 'diff': 0.98, 'diff7d': -0.52, 'ts': 1675485960, 'marketCapUsd': 465473066.69395286, 'availableSupply': 1000000000, 'volume24h': 29561028.70970643, 'volDiff1': -28.05700336322427, 'volDiff7': 21.06923871664246, 'volDiff30': 411.0760211637326, 'diff30d': 84.96641526289207, 'bid': 1.25, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O600" t="n">
@@ -41950,13 +41966,13 @@
         </is>
       </c>
       <c r="H601" t="n">
-        <v>1674736170</v>
+        <v>1675481899</v>
       </c>
       <c r="I601" t="n">
         <v>1</v>
       </c>
       <c r="J601" t="n">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K601" t="inlineStr">
         <is>
@@ -42026,13 +42042,13 @@
         </is>
       </c>
       <c r="H602" t="n">
-        <v>1675048881</v>
+        <v>1675467604</v>
       </c>
       <c r="I602" t="n">
         <v>1257</v>
       </c>
       <c r="J602" t="n">
-        <v>3416</v>
+        <v>3421</v>
       </c>
       <c r="K602" t="inlineStr">
         <is>
@@ -42049,7 +42065,7 @@
       </c>
       <c r="N602" t="inlineStr">
         <is>
-          <t>{'rate': 59.88769428291394, 'diff': 4.55, 'diff7d': -7.14, 'ts': 1675054200, 'marketCapUsd': 1676855.4399215903, 'availableSupply': 28000, 'volume24h': 22219.91793037606, 'volDiff1': 448.00405063359983, 'volDiff7': -51.954390373569595, 'volDiff30': 1013.182630822195, 'bid': 214.95, 'currency': 'USD'}</t>
+          <t>{'rate': 55.595789636936814, 'diff': -0.91, 'diff7d': 5.54, 'ts': 1675482600, 'marketCapUsd': 1556682.1098342307, 'availableSupply': 28000, 'volume24h': 1086.7254627381658, 'volDiff1': -43.79074065977656, 'volDiff7': 66.08453996424873, 'volDiff30': 600.0585737604489, 'bid': 214.95, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O602" t="n">
@@ -42131,7 +42147,7 @@
       </c>
       <c r="N603" t="inlineStr">
         <is>
-          <t>{'rate': 24.104203178547746, 'diff': 0, 'diff7d': -2.91, 'ts': 1675054200, 'marketCapUsd': 337458.84449966846, 'availableSupply': 14000, 'volume24h': 18538.461449155253, 'volDiff1': 177723.3520704289, 'volDiff7': -98.31583368873783, 'volDiff30': 114.37448010934972, 'bid': 29.23, 'currency': 'USD'}</t>
+          <t>{'rate': 24.104203178547746, 'diff': 0, 'diff7d': 0.63, 'ts': 1675360200, 'marketCapUsd': 337458.84449966846, 'availableSupply': 14000, 'volume24h': 16101.928882268145, 'volDiff1': 177723.3520704289, 'volDiff7': -100, 'volDiff30': 288.6325215621143, 'bid': 29.23, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O603" t="n">
@@ -42322,13 +42338,13 @@
       </c>
       <c r="G606" t="inlineStr"/>
       <c r="H606" t="n">
-        <v>1675055059</v>
+        <v>1675485065</v>
       </c>
       <c r="I606" t="n">
         <v>0</v>
       </c>
       <c r="J606" t="n">
-        <v>208227</v>
+        <v>208405</v>
       </c>
       <c r="K606" t="inlineStr">
         <is>
@@ -42345,7 +42361,7 @@
       </c>
       <c r="N606" t="inlineStr">
         <is>
-          <t>{'rate': 56.166995935310354, 'diff': 0.06, 'diff7d': 7.06, 'ts': 1675055760, 'marketCapUsd': 408174096.76247495, 'availableSupply': 7267151.99852569, 'volume24h': 30170944.06362186, 'volDiff1': -9.403416098985701, 'volDiff7': 6.736952394951132, 'volDiff30': 126.62718739960152, 'diff30d': 82.0760903130689, 'bid': 118.74, 'currency': 'USD'}</t>
+          <t>{'rate': 53.57731432705676, 'diff': 1, 'diff7d': -5.8, 'ts': 1675485960, 'marketCapUsd': 389354486.88750964, 'availableSupply': 7267151.99852569, 'volume24h': 31629284.88798352, 'volDiff1': -47.14040058995369, 'volDiff7': 2.0303306438540574, 'volDiff30': 112.04027940351531, 'diff30d': 62.002690445721925, 'bid': 118.74, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O606" t="n">
@@ -42663,7 +42679,7 @@
       </c>
       <c r="F611" t="inlineStr">
         <is>
-          <t>12363207628606734</t>
+          <t>12503354258377914</t>
         </is>
       </c>
       <c r="G611" t="inlineStr">
@@ -42672,13 +42688,13 @@
         </is>
       </c>
       <c r="H611" t="n">
-        <v>1675055384</v>
+        <v>1675485045</v>
       </c>
       <c r="I611" t="n">
-        <v>12462</v>
+        <v>12482</v>
       </c>
       <c r="J611" t="n">
-        <v>12479</v>
+        <v>12653</v>
       </c>
       <c r="K611" t="inlineStr"/>
       <c r="L611" t="inlineStr"/>
@@ -42763,7 +42779,7 @@
       </c>
       <c r="N612" t="inlineStr">
         <is>
-          <t>{'rate': 1.9770378778734746e-05, 'diff': -0.97, 'diff7d': -2.95, 'ts': 1675055460, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 15688.5356579, 'volDiff1': -0.8611144658638494, 'volDiff7': 16.177409982628063, 'volDiff30': 67.52245140986841, 'bid': 4.253e-05, 'currency': 'USD'}</t>
+          <t>{'rate': 2.051004279649499e-05, 'diff': -1.14, 'diff7d': 2.68, 'ts': 1675485660, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 15767.14504165267, 'volDiff1': -0.042242757993847135, 'volDiff7': 17.66483176833684, 'volDiff30': 48.10524742231385, 'bid': 4.253e-05, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O612" t="n">
@@ -42942,7 +42958,7 @@
       </c>
       <c r="G615" t="inlineStr"/>
       <c r="H615" t="n">
-        <v>1674959915</v>
+        <v>1675441363</v>
       </c>
       <c r="I615" t="n">
         <v>3537</v>
@@ -42965,7 +42981,7 @@
       </c>
       <c r="N615" t="inlineStr">
         <is>
-          <t>{'rate': 0.0015227697771870855, 'diff': 7.4, 'diff7d': 14.72, 'ts': 1675055460, 'marketCapUsd': 781734.5483281013, 'availableSupply': 513363582.6238613, 'volume24h': 18084.51681024, 'volDiff1': 23.420719380728045, 'volDiff7': 15.504379475334673, 'volDiff30': 45.35225165194717, 'diff30d': 43.10994831240339, 'bid': 0.00520521, 'currency': 'USD'}</t>
+          <t>{'rate': 0.002016909062063566, 'diff': 22.25, 'diff7d': 39.24, 'ts': 1675485660, 'marketCapUsd': 1035407.6619274841, 'availableSupply': 513363582.6238613, 'volume24h': 23814.264932364345, 'volDiff1': 64.80817530320854, 'volDiff7': 20.80780318392752, 'volDiff30': 36.88681553947063, 'diff30d': 43.10994831240339, 'bid': 0.00520521, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O615" t="n">
@@ -43016,13 +43032,13 @@
       </c>
       <c r="G616" t="inlineStr"/>
       <c r="H616" t="n">
-        <v>1675054453</v>
+        <v>1675481855</v>
       </c>
       <c r="I616" t="n">
         <v>257</v>
       </c>
       <c r="J616" t="n">
-        <v>14062</v>
+        <v>14056</v>
       </c>
       <c r="K616" t="inlineStr">
         <is>
@@ -43039,7 +43055,7 @@
       </c>
       <c r="N616" t="inlineStr">
         <is>
-          <t>{'rate': 48.89607046442521, 'diff': 3.83, 'diff7d': 3.9, 'ts': 1675055460, 'marketCapUsd': 4497592.614256657, 'availableSupply': 91982.70068612, 'volume24h': 66441.92255715141, 'volDiff1': 122.84769166231038, 'volDiff7': -12.651608689474031, 'volDiff30': -73.9622929067048, 'bid': 121.3, 'diff30d': -6.9932705019058545, 'currency': 'USD'}</t>
+          <t>{'rate': 50.59369409179876, 'diff': -4.67, 'diff7d': 8.63, 'ts': 1675485660, 'marketCapUsd': 4653744.620251044, 'availableSupply': 91982.70068612, 'volume24h': 40814.40345244239, 'volDiff1': 52.975574720720914, 'volDiff7': 32.18566012021495, 'volDiff30': -74.37552248113444, 'bid': 121.3, 'diff30d': -6.9932705019058545, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O616" t="n">
@@ -43486,13 +43502,13 @@
       </c>
       <c r="G623" t="inlineStr"/>
       <c r="H623" t="n">
-        <v>1675054808</v>
+        <v>1675484953</v>
       </c>
       <c r="I623" t="n">
         <v>0</v>
       </c>
       <c r="J623" t="n">
-        <v>648459</v>
+        <v>649581</v>
       </c>
       <c r="K623" t="inlineStr">
         <is>
@@ -43509,7 +43525,7 @@
       </c>
       <c r="N623" t="inlineStr">
         <is>
-          <t>{'rate': 7.329416988972341, 'diff': 0.02, 'diff7d': 3.08, 'ts': 1675055760, 'marketCapUsd': 3723343613.8341017, 'availableSupply': 507999970.4527867, 'volume24h': 296125657.07228804, 'volDiff1': 14.234721906681443, 'volDiff7': 6.327050057758484, 'volDiff30': 58.559843765039375, 'diff30d': 33.17161984977969, 'bid': 12.33, 'currency': 'USD'}</t>
+          <t>{'rate': 7.177940445576983, 'diff': 0.92, 'diff7d': -3.33, 'ts': 1675485960, 'marketCapUsd': 3646393534.26497, 'availableSupply': 507999970.4527867, 'volume24h': 265570165.3313536, 'volDiff1': -19.429064362313397, 'volDiff7': -13.324827460547226, 'volDiff30': 81.61645404990597, 'diff30d': 24.947557506951128, 'bid': 12.33, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O623" t="n">
@@ -43844,13 +43860,13 @@
         </is>
       </c>
       <c r="H628" t="n">
-        <v>1675051617</v>
+        <v>1675485230</v>
       </c>
       <c r="I628" t="n">
         <v>1</v>
       </c>
       <c r="J628" t="n">
-        <v>2827</v>
+        <v>2806</v>
       </c>
       <c r="K628" t="inlineStr">
         <is>
@@ -43867,7 +43883,7 @@
       </c>
       <c r="N628" t="inlineStr">
         <is>
-          <t>{'rate': 0.0026038053288442394, 'diff': -2.04, 'diff7d': -26.13, 'ts': 1675055460, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 57898.166156385145, 'volDiff1': 20.055872772757354, 'volDiff7': 52.678992755027025, 'volDiff30': -13.656935662420338, 'diff30d': 897.5493425264311, 'currency': 'USD'}</t>
+          <t>{'rate': 0.0026959602464851173, 'diff': -1.43, 'diff7d': -4.63, 'ts': 1675485660, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 57936.67870674, 'volDiff1': 79.78689311005283, 'volDiff7': -22.39040054393851, 'volDiff30': 6.801788407640856, 'diff30d': 897.5493425264311, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O628" t="n">
@@ -44217,7 +44233,7 @@
       </c>
       <c r="N633" t="inlineStr">
         <is>
-          <t>{'rate': 0.0016730958404100132, 'diff': -1.63, 'diff7d': -90.81, 'ts': 1671187080, 'marketCapUsd': 182367.44660469145, 'availableSupply': 109000000, 'volume24h': 101154.22858818, 'volDiff1': 18676.361596372975, 'volDiff7': -34.58254387101657, 'volDiff30': -99.39637948159776, 'diff30d': -48.54622612703854, 'bid': 0.206392, 'currency': 'USD'}</t>
+          <t>{'rate': 0.0016730958404100132, 'diff': -1.63, 'diff7d': -90.81, 'ts': 1671187080, 'marketCapUsd': 182367.44660469145, 'availableSupply': 109000000, 'volume24h': 101154.22858818, 'volDiff1': 19158.823026018476, 'volDiff7': 31.070602125972158, 'volDiff30': -98.90604028727432, 'diff30d': -48.54622612703854, 'bid': 0.206392, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O633" t="n">
@@ -44472,13 +44488,13 @@
         </is>
       </c>
       <c r="H637" t="n">
-        <v>1675033411</v>
+        <v>1675474104</v>
       </c>
       <c r="I637" t="n">
         <v>1</v>
       </c>
       <c r="J637" t="n">
-        <v>291</v>
+        <v>307</v>
       </c>
       <c r="K637" t="inlineStr">
         <is>
@@ -44495,7 +44511,7 @@
       </c>
       <c r="N637" t="inlineStr">
         <is>
-          <t>{'rate': 0.004458929868966041, 'diff': 22.2, 'diff7d': 11.97, 'ts': 1675054200, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 5527.515386164941, 'volDiff1': -23.69095130108198, 'volDiff7': -59.080830896492465, 'volDiff30': 30.32910100142624, 'currency': 'USD'}</t>
+          <t>{'rate': 0.003805255815308629, 'diff': -7.34, 'diff7d': 5.02, 'ts': 1675482600, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 2968.0388099876513, 'volDiff1': -73.09743206816388, 'volDiff7': 141.22015809542123, 'volDiff30': 154.01205424104765, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O637" t="n">
@@ -44764,7 +44780,9 @@
       </c>
       <c r="K641" t="inlineStr"/>
       <c r="L641" t="inlineStr"/>
-      <c r="M641" t="inlineStr"/>
+      <c r="M641" t="n">
+        <v>0</v>
+      </c>
       <c r="N641" t="b">
         <v>0</v>
       </c>
@@ -45146,13 +45164,13 @@
         </is>
       </c>
       <c r="H647" t="n">
-        <v>1675052770</v>
+        <v>1675485051</v>
       </c>
       <c r="I647" t="n">
         <v>0</v>
       </c>
       <c r="J647" t="n">
-        <v>12507</v>
+        <v>12530</v>
       </c>
       <c r="K647" t="inlineStr">
         <is>
@@ -45169,7 +45187,7 @@
       </c>
       <c r="N647" t="inlineStr">
         <is>
-          <t>{'rate': 0.12435335463749989, 'diff': 3.72, 'diff7d': 8.79, 'ts': 1675055460, 'marketCapUsd': 14220572.621850232, 'availableSupply': 114356164.04, 'volume24h': 813064.05162176, 'volDiff1': 51.68720720193036, 'volDiff7': 28.888923532929397, 'volDiff30': 35.73584483402129, 'diff30d': -20.05539403973583, 'bid': 0.220784, 'currency': 'USD'}</t>
+          <t>{'rate': 0.1418600748776646, 'diff': 0.58, 'diff7d': 20.76, 'ts': 1675485660, 'marketCapUsd': 16222573.993436897, 'availableSupply': 114356164.04, 'volume24h': 758370.37049957, 'volDiff1': -58.43867230810345, 'volDiff7': 93.23252350610827, 'volDiff30': 78.41911642646821, 'diff30d': 36.82613206185172, 'bid': 0.220784, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O647" t="n">
@@ -45224,13 +45242,13 @@
       </c>
       <c r="G648" t="inlineStr"/>
       <c r="H648" t="n">
-        <v>1675054639</v>
+        <v>1675485203</v>
       </c>
       <c r="I648" t="n">
         <v>2</v>
       </c>
       <c r="J648" t="n">
-        <v>152613</v>
+        <v>153045</v>
       </c>
       <c r="K648" t="inlineStr">
         <is>
@@ -45247,7 +45265,7 @@
       </c>
       <c r="N648" t="inlineStr">
         <is>
-          <t>{'rate': 86.38028281492562, 'diff': 0.82, 'diff7d': -0.95, 'ts': 1675055760, 'marketCapUsd': 1217373960.8743808, 'availableSupply': 14093192.58056459, 'volume24h': 83270938.65524659, 'volDiff1': -0.03997010892152275, 'volDiff7': -24.080846818128137, 'volDiff30': 139.1259246543298, 'diff30d': 64.73525623042588, 'bid': 159.53, 'currency': 'USD'}</t>
+          <t>{'rate': 90.06889873977966, 'diff': 1.46, 'diff7d': 2.96, 'ts': 1675485960, 'marketCapUsd': 1269358335.459086, 'availableSupply': 14093192.58056459, 'volume24h': 132586887.71651378, 'volDiff1': -10.857655146144793, 'volDiff7': 2.9476985737540247, 'volDiff30': 178.23019562291836, 'diff30d': 61.343374905936855, 'bid': 159.53, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O648" t="n">
@@ -45384,7 +45402,9 @@
       </c>
       <c r="K650" t="inlineStr"/>
       <c r="L650" t="inlineStr"/>
-      <c r="M650" t="inlineStr"/>
+      <c r="M650" t="n">
+        <v>0</v>
+      </c>
       <c r="N650" t="b">
         <v>0</v>
       </c>
@@ -45508,7 +45528,7 @@
         </is>
       </c>
       <c r="H652" t="n">
-        <v>1675035091</v>
+        <v>1675414124</v>
       </c>
       <c r="I652" t="n">
         <v>0</v>
@@ -45531,7 +45551,7 @@
       </c>
       <c r="N652" t="inlineStr">
         <is>
-          <t>{'rate': 0.6141595889397875, 'diff': 0, 'diff7d': 1.83, 'ts': 1675054200, 'marketCapUsd': 2238778.881222675, 'availableSupply': 3645272.20862486, 'volume24h': 0, 'volDiff1': -96.15594909121074, 'volDiff7': -28.10045653579691, 'volDiff30': -99.4805614451015, 'bid': 0.737626, 'currency': 'USD'}</t>
+          <t>{'rate': 0.6040727667712946, 'diff': -9.18, 'diff7d': -1.64, 'ts': 1675482600, 'marketCapUsd': 2202009.668698527, 'availableSupply': 3645272.20862486, 'volume24h': 3760.55814778, 'volDiff1': 408.7587517120709, 'volDiff7': 261.7076181953, 'volDiff30': -98.25080042235281, 'bid': 0.737626, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O652" t="n">
@@ -45961,18 +45981,18 @@
       </c>
       <c r="F659" t="inlineStr">
         <is>
-          <t>635287317022533004637639</t>
+          <t>635287133544367182425335</t>
         </is>
       </c>
       <c r="G659" t="inlineStr"/>
       <c r="H659" t="n">
-        <v>1675049858</v>
+        <v>1675482851</v>
       </c>
       <c r="I659" t="n">
-        <v>20250</v>
+        <v>20318</v>
       </c>
       <c r="J659" t="n">
-        <v>25466</v>
+        <v>25472</v>
       </c>
       <c r="K659" t="inlineStr">
         <is>
@@ -45989,7 +46009,7 @@
       </c>
       <c r="N659" t="inlineStr">
         <is>
-          <t>{'rate': 0.542410566654195, 'diff': 0.76, 'diff7d': 15.52, 'ts': 1675055460, 'marketCapUsd': 26184075.60758246, 'availableSupply': 48273535.2467344, 'volume24h': 567161.68201064, 'volDiff1': -21.05020287128258, 'volDiff7': 59.585741334240026, 'volDiff30': -25.371773618556276, 'diff30d': -16.536056899128383, 'bid': 0.910911, 'currency': 'USD'}</t>
+          <t>{'rate': 0.5391927076081208, 'diff': -1.78, 'diff7d': 1.06, 'ts': 1675485660, 'marketCapUsd': 26028738.175502773, 'availableSupply': 48273535.2467344, 'volume24h': 572477.36530744, 'volDiff1': -16.151585395189656, 'volDiff7': 27.766217706495368, 'volDiff30': -5.019643101641265, 'diff30d': -16.536056899128383, 'bid': 0.910911, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O659" t="n">
@@ -46420,13 +46440,13 @@
       </c>
       <c r="G666" t="inlineStr"/>
       <c r="H666" t="n">
-        <v>1675002321</v>
+        <v>1675467306</v>
       </c>
       <c r="I666" t="n">
         <v>2</v>
       </c>
       <c r="J666" t="n">
-        <v>6723</v>
+        <v>6733</v>
       </c>
       <c r="K666" t="inlineStr">
         <is>
@@ -46443,7 +46463,7 @@
       </c>
       <c r="N666" t="inlineStr">
         <is>
-          <t>{'rate': 0.29424141660160436, 'diff': 3.1, 'diff7d': 3.25, 'ts': 1675054200, 'marketCapUsd': 6996131.789941478, 'availableSupply': 0, 'volume24h': 328.82143948, 'volDiff1': -94.61307335075793, 'volDiff7': 67.2414689135826, 'volDiff30': -55.99037066739171, 'bid': 0.970516, 'diff30d': -18.539308310648707, 'currency': 'USD'}</t>
+          <t>{'rate': 0.24756103686346784, 'diff': -13.47, 'diff7d': -8.28, 'ts': 1675482600, 'marketCapUsd': 5877202.586250835, 'availableSupply': 0, 'volume24h': 2527.03734922, 'volDiff1': 81.65226714924455, 'volDiff7': 133.73299603947632, 'volDiff30': -27.114369303787186, 'bid': 0.970516, 'diff30d': -18.539308310648707, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O666" t="n">
@@ -46504,7 +46524,9 @@
       </c>
       <c r="K667" t="inlineStr"/>
       <c r="L667" t="inlineStr"/>
-      <c r="M667" t="inlineStr"/>
+      <c r="M667" t="n">
+        <v>0</v>
+      </c>
       <c r="N667" t="b">
         <v>0</v>
       </c>
@@ -47296,7 +47318,9 @@
       </c>
       <c r="K679" t="inlineStr"/>
       <c r="L679" t="inlineStr"/>
-      <c r="M679" t="inlineStr"/>
+      <c r="M679" t="n">
+        <v>0</v>
+      </c>
       <c r="N679" t="b">
         <v>0</v>
       </c>
@@ -47742,7 +47766,9 @@
       </c>
       <c r="K686" t="inlineStr"/>
       <c r="L686" t="inlineStr"/>
-      <c r="M686" t="inlineStr"/>
+      <c r="M686" t="n">
+        <v>0</v>
+      </c>
       <c r="N686" t="b">
         <v>0</v>
       </c>
@@ -48064,7 +48090,9 @@
       </c>
       <c r="K691" t="inlineStr"/>
       <c r="L691" t="inlineStr"/>
-      <c r="M691" t="inlineStr"/>
+      <c r="M691" t="n">
+        <v>0</v>
+      </c>
       <c r="N691" t="b">
         <v>0</v>
       </c>
@@ -48516,7 +48544,9 @@
       </c>
       <c r="K698" t="inlineStr"/>
       <c r="L698" t="inlineStr"/>
-      <c r="M698" t="inlineStr"/>
+      <c r="M698" t="n">
+        <v>0</v>
+      </c>
       <c r="N698" t="b">
         <v>0</v>
       </c>
@@ -48677,11 +48707,7 @@
           <t>Voyager Pass</t>
         </is>
       </c>
-      <c r="D701" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="D701" t="inlineStr"/>
       <c r="E701" t="inlineStr">
         <is>
           <t>VOP</t>
@@ -48689,7 +48715,7 @@
       </c>
       <c r="F701" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2033</t>
         </is>
       </c>
       <c r="G701" t="inlineStr">
@@ -48698,13 +48724,13 @@
         </is>
       </c>
       <c r="H701" t="n">
-        <v>1674815923</v>
+        <v>1675483860</v>
       </c>
       <c r="I701" t="n">
         <v>0</v>
       </c>
       <c r="J701" t="n">
-        <v>1842</v>
+        <v>1787</v>
       </c>
       <c r="K701" t="inlineStr"/>
       <c r="L701" t="inlineStr"/>
@@ -48832,13 +48858,13 @@
         </is>
       </c>
       <c r="H703" t="n">
-        <v>1675054191</v>
+        <v>1675463358</v>
       </c>
       <c r="I703" t="n">
         <v>4</v>
       </c>
       <c r="J703" t="n">
-        <v>5129</v>
+        <v>5138</v>
       </c>
       <c r="K703" t="inlineStr">
         <is>
@@ -48855,11 +48881,11 @@
       </c>
       <c r="N703" t="inlineStr">
         <is>
-          <t>{'rate': 6.110520639539712e-05, 'diff': 10.34, 'diff7d': -10.91, 'ts': 1675054200, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 7452.668857180883, 'volDiff1': 132.9019606999414, 'volDiff7': 93.21811024450716, 'volDiff30': -45.340979983369515, 'currency': 'USD'}</t>
+          <t>{'rate': 5.95805392940638e-05, 'diff': -0.45, 'diff7d': 6.54, 'ts': 1675482600, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 3723.682066842435, 'volDiff1': 75.77638366529936, 'volDiff7': -4.324556631752756, 'volDiff30': -33.73243382112125, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O703" t="n">
-        <v>1.14307561692363e+26</v>
+        <v>1.143916430036553e+26</v>
       </c>
       <c r="P703" t="n">
         <v>0</v>
@@ -48869,7 +48895,7 @@
       </c>
       <c r="R703" t="inlineStr">
         <is>
-          <t>114307561692363051527828551</t>
+          <t>114391643003655324427490547</t>
         </is>
       </c>
       <c r="S703" t="inlineStr"/>
@@ -49492,13 +49518,13 @@
       </c>
       <c r="G713" t="inlineStr"/>
       <c r="H713" t="n">
-        <v>1675017672</v>
+        <v>1675340763</v>
       </c>
       <c r="I713" t="n">
         <v>1</v>
       </c>
       <c r="J713" t="n">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="K713" t="inlineStr"/>
       <c r="L713" t="inlineStr"/>
@@ -49636,7 +49662,9 @@
       </c>
       <c r="K715" t="inlineStr"/>
       <c r="L715" t="inlineStr"/>
-      <c r="M715" t="inlineStr"/>
+      <c r="M715" t="n">
+        <v>0</v>
+      </c>
       <c r="N715" t="b">
         <v>0</v>
       </c>
@@ -49896,7 +49924,9 @@
       </c>
       <c r="K719" t="inlineStr"/>
       <c r="L719" t="inlineStr"/>
-      <c r="M719" t="inlineStr"/>
+      <c r="M719" t="n">
+        <v>0</v>
+      </c>
       <c r="N719" t="b">
         <v>0</v>
       </c>
@@ -50282,13 +50312,13 @@
         </is>
       </c>
       <c r="H725" t="n">
-        <v>1675038627</v>
+        <v>1675319048</v>
       </c>
       <c r="I725" t="n">
         <v>1</v>
       </c>
       <c r="J725" t="n">
-        <v>1136</v>
+        <v>1138</v>
       </c>
       <c r="K725" t="inlineStr"/>
       <c r="L725" t="inlineStr"/>
@@ -50558,7 +50588,9 @@
       </c>
       <c r="K729" t="inlineStr"/>
       <c r="L729" t="inlineStr"/>
-      <c r="M729" t="inlineStr"/>
+      <c r="M729" t="n">
+        <v>0</v>
+      </c>
       <c r="N729" t="b">
         <v>0</v>
       </c>
@@ -50688,7 +50720,9 @@
       </c>
       <c r="K731" t="inlineStr"/>
       <c r="L731" t="inlineStr"/>
-      <c r="M731" t="inlineStr"/>
+      <c r="M731" t="n">
+        <v>0</v>
+      </c>
       <c r="N731" t="b">
         <v>0</v>
       </c>
@@ -50744,17 +50778,19 @@
         </is>
       </c>
       <c r="H732" t="n">
-        <v>1675054634</v>
+        <v>1675485837</v>
       </c>
       <c r="I732" t="n">
         <v>1</v>
       </c>
       <c r="J732" t="n">
-        <v>1067</v>
+        <v>1224</v>
       </c>
       <c r="K732" t="inlineStr"/>
       <c r="L732" t="inlineStr"/>
-      <c r="M732" t="inlineStr"/>
+      <c r="M732" t="n">
+        <v>0</v>
+      </c>
       <c r="N732" t="b">
         <v>0</v>
       </c>
@@ -50956,7 +50992,9 @@
       </c>
       <c r="K735" t="inlineStr"/>
       <c r="L735" t="inlineStr"/>
-      <c r="M735" t="inlineStr"/>
+      <c r="M735" t="n">
+        <v>0</v>
+      </c>
       <c r="N735" t="b">
         <v>0</v>
       </c>
@@ -51018,7 +51056,9 @@
       </c>
       <c r="K736" t="inlineStr"/>
       <c r="L736" t="inlineStr"/>
-      <c r="M736" t="inlineStr"/>
+      <c r="M736" t="n">
+        <v>0</v>
+      </c>
       <c r="N736" t="b">
         <v>0</v>
       </c>
@@ -51329,24 +51369,22 @@
       </c>
       <c r="F741" t="inlineStr">
         <is>
-          <t>29835478292650000001086396737</t>
+          <t>29835584292650000001086396737</t>
         </is>
       </c>
       <c r="G741" t="inlineStr"/>
       <c r="H741" t="n">
-        <v>1675017333</v>
+        <v>1675442859</v>
       </c>
       <c r="I741" t="n">
-        <v>2776</v>
+        <v>2783</v>
       </c>
       <c r="J741" t="n">
-        <v>6639</v>
+        <v>6643</v>
       </c>
       <c r="K741" t="inlineStr"/>
       <c r="L741" t="inlineStr"/>
-      <c r="M741" t="n">
-        <v>0</v>
-      </c>
+      <c r="M741" t="inlineStr"/>
       <c r="N741" t="b">
         <v>0</v>
       </c>
@@ -51460,13 +51498,13 @@
       </c>
       <c r="G743" t="inlineStr"/>
       <c r="H743" t="n">
-        <v>1674981274</v>
+        <v>1675472733</v>
       </c>
       <c r="I743" t="n">
         <v>1</v>
       </c>
       <c r="J743" t="n">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="K743" t="inlineStr"/>
       <c r="L743" t="inlineStr"/>
@@ -52128,7 +52166,9 @@
       </c>
       <c r="K753" t="inlineStr"/>
       <c r="L753" t="inlineStr"/>
-      <c r="M753" t="inlineStr"/>
+      <c r="M753" t="n">
+        <v>0</v>
+      </c>
       <c r="N753" t="b">
         <v>0</v>
       </c>
@@ -52650,13 +52690,13 @@
         </is>
       </c>
       <c r="H761" t="n">
-        <v>1675055691</v>
+        <v>1675485878</v>
       </c>
       <c r="I761" t="n">
         <v>1</v>
       </c>
       <c r="J761" t="n">
-        <v>1703</v>
+        <v>1740</v>
       </c>
       <c r="K761" t="inlineStr">
         <is>
@@ -52668,10 +52708,12 @@
           <t>/images/DBI2de509bf.png</t>
         </is>
       </c>
-      <c r="M761" t="inlineStr"/>
+      <c r="M761" t="n">
+        <v>0</v>
+      </c>
       <c r="N761" t="inlineStr">
         <is>
-          <t>{'rate': 0.003660618978319737, 'diff': 52.93, 'diff7d': 26.76, 'ts': 1675055460, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 272641.1543055349, 'volDiff1': 286.01785229009533, 'volDiff7': 137.9939487143967, 'volDiff30': -91.61409207920269, 'diff30d': -25.08214374409387, 'currency': 'USD'}</t>
+          <t>{'rate': 0.002756119482372122, 'diff': -7.66, 'diff7d': 9.22, 'ts': 1675485960, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 6058380.45617134, 'volDiff1': 469.9853067402645, 'volDiff7': 7226.322578250152, 'volDiff30': -23.090568400720727, 'diff30d': 14.20721131645277, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O761" t="n">
@@ -52868,7 +52910,9 @@
       </c>
       <c r="K764" t="inlineStr"/>
       <c r="L764" t="inlineStr"/>
-      <c r="M764" t="inlineStr"/>
+      <c r="M764" t="n">
+        <v>0</v>
+      </c>
       <c r="N764" t="b">
         <v>0</v>
       </c>
@@ -52915,7 +52959,7 @@
       </c>
       <c r="F765" t="inlineStr">
         <is>
-          <t>351238601007758925137332040</t>
+          <t>350990906124809938030584241</t>
         </is>
       </c>
       <c r="G765" t="inlineStr">
@@ -52924,13 +52968,13 @@
         </is>
       </c>
       <c r="H765" t="n">
-        <v>1675047487</v>
+        <v>1675485783</v>
       </c>
       <c r="I765" t="n">
-        <v>1448</v>
+        <v>1476</v>
       </c>
       <c r="J765" t="n">
-        <v>461</v>
+        <v>471</v>
       </c>
       <c r="K765" t="inlineStr">
         <is>
@@ -52947,7 +52991,7 @@
       </c>
       <c r="N765" t="inlineStr">
         <is>
-          <t>{'rate': 0.002106783810779875, 'diff': 6.59, 'diff7d': -7.83, 'ts': 1675054200, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 6671.181449254995, 'volDiff1': 63.7032035205126, 'volDiff7': -65.37099080478238, 'volDiff30': -39.131051122969, 'currency': 'USD'}</t>
+          <t>{'rate': 0.002199106302380615, 'diff': -5.74, 'diff7d': 9.51, 'ts': 1675482600, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 5892.85904458, 'volDiff1': 3.6768489890253875, 'volDiff7': 92.63754162917269, 'volDiff30': -3.79792796198943, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O765" t="n">
@@ -53266,13 +53310,13 @@
       </c>
       <c r="G770" t="inlineStr"/>
       <c r="H770" t="n">
-        <v>1674869328</v>
+        <v>1675235780</v>
       </c>
       <c r="I770" t="n">
         <v>1</v>
       </c>
       <c r="J770" t="n">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="K770" t="inlineStr"/>
       <c r="L770" t="inlineStr"/>
@@ -53476,7 +53520,9 @@
       </c>
       <c r="K773" t="inlineStr"/>
       <c r="L773" t="inlineStr"/>
-      <c r="M773" t="inlineStr"/>
+      <c r="M773" t="n">
+        <v>0</v>
+      </c>
       <c r="N773" t="b">
         <v>0</v>
       </c>
@@ -53532,7 +53578,7 @@
         </is>
       </c>
       <c r="H774" t="n">
-        <v>1674944778</v>
+        <v>1675084031</v>
       </c>
       <c r="I774" t="n">
         <v>1</v>
@@ -54122,7 +54168,9 @@
       </c>
       <c r="K783" t="inlineStr"/>
       <c r="L783" t="inlineStr"/>
-      <c r="M783" t="inlineStr"/>
+      <c r="M783" t="n">
+        <v>0</v>
+      </c>
       <c r="N783" t="b">
         <v>0</v>
       </c>
@@ -54448,7 +54496,9 @@
       </c>
       <c r="K788" t="inlineStr"/>
       <c r="L788" t="inlineStr"/>
-      <c r="M788" t="inlineStr"/>
+      <c r="M788" t="n">
+        <v>0</v>
+      </c>
       <c r="N788" t="b">
         <v>0</v>
       </c>
@@ -54514,7 +54564,9 @@
       </c>
       <c r="K789" t="inlineStr"/>
       <c r="L789" t="inlineStr"/>
-      <c r="M789" t="inlineStr"/>
+      <c r="M789" t="n">
+        <v>0</v>
+      </c>
       <c r="N789" t="b">
         <v>0</v>
       </c>
@@ -54937,7 +54989,7 @@
       </c>
       <c r="F796" t="inlineStr">
         <is>
-          <t>1102000000000000000000000</t>
+          <t>1109000000000000000000000</t>
         </is>
       </c>
       <c r="G796" t="inlineStr">
@@ -54946,10 +54998,10 @@
         </is>
       </c>
       <c r="H796" t="n">
-        <v>1674864945</v>
+        <v>1675469763</v>
       </c>
       <c r="I796" t="n">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="J796" t="n">
         <v>68</v>
@@ -55014,13 +55066,13 @@
         </is>
       </c>
       <c r="H797" t="n">
-        <v>1674184623</v>
+        <v>1675402898</v>
       </c>
       <c r="I797" t="n">
         <v>1</v>
       </c>
       <c r="J797" t="n">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K797" t="inlineStr"/>
       <c r="L797" t="inlineStr"/>
@@ -55092,7 +55144,9 @@
       </c>
       <c r="K798" t="inlineStr"/>
       <c r="L798" t="inlineStr"/>
-      <c r="M798" t="inlineStr"/>
+      <c r="M798" t="n">
+        <v>0</v>
+      </c>
       <c r="N798" t="b">
         <v>0</v>
       </c>
@@ -55144,13 +55198,13 @@
       </c>
       <c r="G799" t="inlineStr"/>
       <c r="H799" t="n">
-        <v>1674967965</v>
+        <v>1675419326</v>
       </c>
       <c r="I799" t="n">
         <v>0</v>
       </c>
       <c r="J799" t="n">
-        <v>19077</v>
+        <v>19078</v>
       </c>
       <c r="K799" t="inlineStr"/>
       <c r="L799" t="inlineStr"/>
@@ -55212,13 +55266,13 @@
         </is>
       </c>
       <c r="H800" t="n">
-        <v>1675054971</v>
+        <v>1675484961</v>
       </c>
       <c r="I800" t="n">
-        <v>1502157</v>
+        <v>1503467</v>
       </c>
       <c r="J800" t="n">
-        <v>69698</v>
+        <v>70801</v>
       </c>
       <c r="K800" t="inlineStr">
         <is>
@@ -55235,7 +55289,7 @@
       </c>
       <c r="N800" t="inlineStr">
         <is>
-          <t>{'rate': 1.3543927413029675, 'diff': 1.46, 'diff7d': -4.05, 'ts': 1675055760, 'marketCapUsd': 222880714.00424793, 'availableSupply': 164561361.86157483, 'volume24h': 4730012.59141476, 'volDiff1': 24.550323597783816, 'volDiff7': -51.35805958740161, 'volDiff30': 65.77513100587896, 'diff30d': 56.635796890222764, 'bid': 0.554829, 'currency': 'USD'}</t>
+          <t>{'rate': 1.6650051280223825, 'diff': 10.9, 'diff7d': 22.01, 'ts': 1675485960, 'marketCapUsd': 277409460.7734556, 'availableSupply': 166611775.606331, 'volume24h': 15330431.07370386, 'volDiff1': 53.26500723976952, 'volDiff7': 29.196613847025645, 'volDiff30': 85.08299976535596, 'diff30d': 59.73541931973443, 'bid': 0.554829, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O800" t="n">
@@ -55286,13 +55340,13 @@
       </c>
       <c r="G801" t="inlineStr"/>
       <c r="H801" t="n">
-        <v>1675053969</v>
+        <v>1675482223</v>
       </c>
       <c r="I801" t="n">
         <v>6</v>
       </c>
       <c r="J801" t="n">
-        <v>4903</v>
+        <v>4924</v>
       </c>
       <c r="K801" t="inlineStr">
         <is>
@@ -55309,7 +55363,7 @@
       </c>
       <c r="N801" t="inlineStr">
         <is>
-          <t>{'rate': 0.0028887268334651123, 'diff': -1.26, 'diff7d': 2.53, 'ts': 1675055760, 'marketCapUsd': 8829746.616626933, 'availableSupply': 3056622216.52, 'volume24h': 1246191.49268779, 'volDiff1': -10.008781921002878, 'volDiff7': 7.076688734866977, 'volDiff30': -29.52888672851074, 'diff30d': 26.47815210361115, 'bid': 0.293665, 'currency': 'USD'}</t>
+          <t>{'rate': 0.0031364101641935312, 'diff': 2.37, 'diff7d': 8.22, 'ts': 1675485960, 'marketCapUsd': 9586820.987993088, 'availableSupply': 3056622216.52, 'volume24h': 3515764.48872527, 'volDiff1': -31.967860762863126, 'volDiff7': 26.699132333352523, 'volDiff30': -3.1165741527797763, 'diff30d': 35.0884323586688, 'bid': 0.293665, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O801" t="n">
@@ -55492,13 +55546,13 @@
         </is>
       </c>
       <c r="H804" t="n">
-        <v>1675055702</v>
+        <v>1675483741</v>
       </c>
       <c r="I804" t="n">
         <v>1</v>
       </c>
       <c r="J804" t="n">
-        <v>1884</v>
+        <v>1894</v>
       </c>
       <c r="K804" t="inlineStr">
         <is>
@@ -55515,7 +55569,7 @@
       </c>
       <c r="N804" t="inlineStr">
         <is>
-          <t>{'rate': 0.7270237955442174, 'diff': 43.53, 'diff7d': 44.26, 'ts': 1675055760, 'marketCapUsd': 7031960.369211138, 'availableSupply': 0, 'volume24h': 1523707.57102373, 'volDiff1': 31.096144843233986, 'volDiff7': 7.25406673015803, 'volDiff30': 4.726220201534531, 'diff30d': 36.774720617996906, 'currency': 'USD'}</t>
+          <t>{'rate': 0.6183669927915478, 'diff': -8.41, 'diff7d': 6.72, 'ts': 1675485660, 'marketCapUsd': 6132968.920088261, 'availableSupply': 0, 'volume24h': 709868.90584058, 'volDiff1': -38.46606862169432, 'volDiff7': 20.43026287712793, 'volDiff30': 7.0242069329868, 'diff30d': 66.74006293693819, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O804" t="n">
@@ -55702,13 +55756,13 @@
         </is>
       </c>
       <c r="H807" t="n">
-        <v>1675042449</v>
+        <v>1675439834</v>
       </c>
       <c r="I807" t="n">
         <v>1</v>
       </c>
       <c r="J807" t="n">
-        <v>6957</v>
+        <v>6952</v>
       </c>
       <c r="K807" t="inlineStr">
         <is>
@@ -55725,7 +55779,7 @@
       </c>
       <c r="N807" t="inlineStr">
         <is>
-          <t>{'rate': 0.28254309491300106, 'diff': 12.47, 'diff7d': -16.57, 'ts': 1675055460, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 28824.37594786, 'volDiff1': -8.028195006652126, 'volDiff7': 0.048034972007386045, 'volDiff30': -37.67514771535372, 'currency': 'USD'}</t>
+          <t>{'rate': 0.25964007145764034, 'diff': -0.28, 'diff7d': -0.88, 'ts': 1675482600, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 847.3629745172573, 'volDiff1': -93.30797563327049, 'volDiff7': 159.9199414860696, 'volDiff30': -15.99687599239489, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O807" t="n">
@@ -56242,7 +56296,9 @@
       </c>
       <c r="K815" t="inlineStr"/>
       <c r="L815" t="inlineStr"/>
-      <c r="M815" t="inlineStr"/>
+      <c r="M815" t="n">
+        <v>0</v>
+      </c>
       <c r="N815" t="b">
         <v>0</v>
       </c>
@@ -56942,13 +56998,13 @@
         </is>
       </c>
       <c r="H826" t="n">
-        <v>1675038152</v>
+        <v>1675476155</v>
       </c>
       <c r="I826" t="n">
         <v>1</v>
       </c>
       <c r="J826" t="n">
-        <v>1237</v>
+        <v>1229</v>
       </c>
       <c r="K826" t="inlineStr">
         <is>
@@ -56965,7 +57021,7 @@
       </c>
       <c r="N826" t="inlineStr">
         <is>
-          <t>{'rate': 0.007141480460393102, 'diff': -0.52, 'diff7d': 2.29, 'ts': 1675054200, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 1146.1030460652578, 'volDiff1': -77.99899820226041, 'volDiff7': -0.02749728564964471, 'volDiff30': -30.423345929703927, 'currency': 'USD'}</t>
+          <t>{'rate': 0.0059692964310742065, 'diff': -12.15, 'diff7d': -3.88, 'ts': 1675482600, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 4730.489614266835, 'volDiff1': 116.88069270545563, 'volDiff7': -68.01578054302163, 'volDiff30': -35.00318718691396, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O826" t="n">
@@ -57152,13 +57208,13 @@
       </c>
       <c r="G829" t="inlineStr"/>
       <c r="H829" t="n">
-        <v>1674998338</v>
+        <v>1675441080</v>
       </c>
       <c r="I829" t="n">
         <v>0</v>
       </c>
       <c r="J829" t="n">
-        <v>5756</v>
+        <v>5759</v>
       </c>
       <c r="K829" t="inlineStr">
         <is>
@@ -57175,7 +57231,7 @@
       </c>
       <c r="N829" t="inlineStr">
         <is>
-          <t>{'rate': 0.0019945555243229213, 'diff': -7.57, 'diff7d': 8.95, 'ts': 1675055460, 'marketCapUsd': 461099.7939286686, 'availableSupply': 231179221.78937343, 'volume24h': 23754.34406145958, 'volDiff1': 15.959251909687893, 'volDiff7': -17.82748924972924, 'volDiff30': 17.576847690107257, 'diff30d': 43.57746114389042, 'bid': 0.00596363, 'currency': 'USD'}</t>
+          <t>{'rate': 0.0019778295217137464, 'diff': 0.17, 'diff7d': -3.13, 'ts': 1675485660, 'marketCapUsd': 457233.08966183255, 'availableSupply': 231179221.78937343, 'volume24h': 25759.429427053703, 'volDiff1': -0.16544084411538051, 'volDiff7': 19.08399858711229, 'volDiff30': 16.605825126391196, 'diff30d': 43.57746114389042, 'bid': 0.00596363, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O829" t="n">
@@ -57221,7 +57277,7 @@
       </c>
       <c r="F830" t="inlineStr">
         <is>
-          <t>828332080000000000000000000</t>
+          <t>831188560000000000000000000</t>
         </is>
       </c>
       <c r="G830" t="inlineStr">
@@ -57230,13 +57286,13 @@
         </is>
       </c>
       <c r="H830" t="n">
-        <v>1675055474</v>
+        <v>1675485366</v>
       </c>
       <c r="I830" t="n">
-        <v>637341</v>
+        <v>639501</v>
       </c>
       <c r="J830" t="n">
-        <v>69040</v>
+        <v>69290</v>
       </c>
       <c r="K830" t="inlineStr">
         <is>
@@ -57253,7 +57309,7 @@
       </c>
       <c r="N830" t="inlineStr">
         <is>
-          <t>{'rate': 0.2056851709017374, 'diff': -0.06, 'diff7d': -5.61, 'ts': 1675055760, 'marketCapUsd': 96577220.12994912, 'availableSupply': 469539051.875, 'volume24h': 5720005.9772787, 'volDiff1': 22.346219087631965, 'volDiff7': -31.845843175632467, 'volDiff30': 30.998466967582516, 'diff30d': 43.7455249586902, 'bid': 1.44, 'currency': 'USD'}</t>
+          <t>{'rate': 0.28400879730982526, 'diff': 19.03, 'diff7d': 34.39, 'ts': 1675485960, 'marketCapUsd': 133353221.4130144, 'availableSupply': 469539051.875, 'volume24h': 50422389.83415571, 'volDiff1': 102.36808535354504, 'volDiff7': 206.3909719524624, 'volDiff30': 117.52272113431465, 'diff30d': 74.86244099265733, 'bid': 1.44, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O830" t="n">
@@ -57308,13 +57364,13 @@
         </is>
       </c>
       <c r="H831" t="n">
-        <v>1674996746</v>
+        <v>1675397917</v>
       </c>
       <c r="I831" t="n">
         <v>1</v>
       </c>
       <c r="J831" t="n">
-        <v>511</v>
+        <v>516</v>
       </c>
       <c r="K831" t="inlineStr"/>
       <c r="L831" t="inlineStr"/>
@@ -57323,11 +57379,11 @@
       </c>
       <c r="N831" t="inlineStr">
         <is>
-          <t>{'rate': 1.460323717724029e-07, 'diff': 1.45, 'diff7d': 1.27, 'ts': 1675054200, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 104.92700173186272, 'volDiff1': -87.11277898717493, 'volDiff7': 261.7981410757023, 'volDiff30': -18.19089595059019, 'currency': 'USD'}</t>
+          <t>{'rate': 1.393454318945031e-07, 'diff': -1.8, 'diff7d': 0.8, 'ts': 1675482600, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 1078.7125543101834, 'volDiff1': 224.87101712934555, 'volDiff7': 210.63759934772548, 'volDiff30': 60.373644794074295, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O831" t="n">
-        <v>6.671646092552572e+16</v>
+        <v>6.67395908215725e+16</v>
       </c>
       <c r="P831" t="n">
         <v>0</v>
@@ -57337,7 +57393,7 @@
       </c>
       <c r="R831" t="inlineStr">
         <is>
-          <t>66716460925525720</t>
+          <t>66739590821572504</t>
         </is>
       </c>
       <c r="S831" t="inlineStr"/>
@@ -57378,17 +57434,19 @@
         </is>
       </c>
       <c r="H832" t="n">
-        <v>1673813842</v>
+        <v>1675241276</v>
       </c>
       <c r="I832" t="n">
         <v>1</v>
       </c>
       <c r="J832" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K832" t="inlineStr"/>
       <c r="L832" t="inlineStr"/>
-      <c r="M832" t="inlineStr"/>
+      <c r="M832" t="n">
+        <v>0</v>
+      </c>
       <c r="N832" t="b">
         <v>0</v>
       </c>
@@ -57712,7 +57770,9 @@
       </c>
       <c r="K837" t="inlineStr"/>
       <c r="L837" t="inlineStr"/>
-      <c r="M837" t="inlineStr"/>
+      <c r="M837" t="n">
+        <v>0</v>
+      </c>
       <c r="N837" t="b">
         <v>0</v>
       </c>
@@ -57836,19 +57896,17 @@
         </is>
       </c>
       <c r="H839" t="n">
-        <v>1674908027</v>
+        <v>1675479146</v>
       </c>
       <c r="I839" t="n">
         <v>1</v>
       </c>
       <c r="J839" t="n">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="K839" t="inlineStr"/>
       <c r="L839" t="inlineStr"/>
-      <c r="M839" t="n">
-        <v>0</v>
-      </c>
+      <c r="M839" t="inlineStr"/>
       <c r="N839" t="b">
         <v>0</v>
       </c>
@@ -58036,13 +58094,13 @@
         </is>
       </c>
       <c r="H842" t="n">
-        <v>1674939577</v>
+        <v>1675323941</v>
       </c>
       <c r="I842" t="n">
         <v>1</v>
       </c>
       <c r="J842" t="n">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="K842" t="inlineStr"/>
       <c r="L842" t="inlineStr"/>
@@ -58114,7 +58172,9 @@
       </c>
       <c r="K843" t="inlineStr"/>
       <c r="L843" t="inlineStr"/>
-      <c r="M843" t="inlineStr"/>
+      <c r="M843" t="n">
+        <v>0</v>
+      </c>
       <c r="N843" t="b">
         <v>0</v>
       </c>
@@ -58430,13 +58490,13 @@
         </is>
       </c>
       <c r="H848" t="n">
-        <v>1675031270</v>
+        <v>1675464663</v>
       </c>
       <c r="I848" t="n">
         <v>1</v>
       </c>
       <c r="J848" t="n">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="K848" t="inlineStr"/>
       <c r="L848" t="inlineStr"/>
@@ -58572,7 +58632,9 @@
       </c>
       <c r="K850" t="inlineStr"/>
       <c r="L850" t="inlineStr"/>
-      <c r="M850" t="inlineStr"/>
+      <c r="M850" t="n">
+        <v>0</v>
+      </c>
       <c r="N850" t="b">
         <v>0</v>
       </c>
@@ -59016,13 +59078,13 @@
       </c>
       <c r="G857" t="inlineStr"/>
       <c r="H857" t="n">
-        <v>1675023732</v>
+        <v>1675303844</v>
       </c>
       <c r="I857" t="n">
         <v>4</v>
       </c>
       <c r="J857" t="n">
-        <v>13052</v>
+        <v>13055</v>
       </c>
       <c r="K857" t="inlineStr">
         <is>
@@ -59039,7 +59101,7 @@
       </c>
       <c r="N857" t="inlineStr">
         <is>
-          <t>{'rate': 0.43701318135010425, 'diff': -1.72, 'diff7d': -0.33, 'ts': 1675055460, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 206021.52270399593, 'volDiff1': 14.718983859519, 'volDiff7': 30.84974284822877, 'volDiff30': 3.2902551772323108, 'currency': 'USD'}</t>
+          <t>{'rate': 0.4348803642313481, 'diff': -2.48, 'diff7d': -1.67, 'ts': 1675485660, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 165976.53789808005, 'volDiff1': 3.6247211142072615, 'volDiff7': 20.791439460374676, 'volDiff30': 12.892793433983513, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O857" t="n">
@@ -59162,13 +59224,13 @@
         </is>
       </c>
       <c r="H859" t="n">
-        <v>1675055573</v>
+        <v>1675484265</v>
       </c>
       <c r="I859" t="n">
         <v>0</v>
       </c>
       <c r="J859" t="n">
-        <v>1654</v>
+        <v>1662</v>
       </c>
       <c r="K859" t="inlineStr">
         <is>
@@ -59185,7 +59247,7 @@
       </c>
       <c r="N859" t="inlineStr">
         <is>
-          <t>{'rate': 0.00031223564178423064, 'diff': 10.6, 'diff7d': -2.02, 'ts': 1675055460, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 138066.02493883, 'volDiff1': 58.81407372004213, 'volDiff7': 19.50815286528224, 'volDiff30': 12.354836714002232, 'currency': 'USD'}</t>
+          <t>{'rate': 0.0002946636399234093, 'diff': -7.73, 'diff7d': 13.55, 'ts': 1675485660, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 124322.6260716, 'volDiff1': -11.732030048814963, 'volDiff7': 1.2857992158362208, 'volDiff30': 11.627393248645575, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O859" t="n">
@@ -59304,13 +59366,13 @@
         </is>
       </c>
       <c r="H861" t="n">
-        <v>1675055010</v>
+        <v>1675479621</v>
       </c>
       <c r="I861" t="n">
         <v>1</v>
       </c>
       <c r="J861" t="n">
-        <v>68034</v>
+        <v>68030</v>
       </c>
       <c r="K861" t="inlineStr">
         <is>
@@ -59327,11 +59389,11 @@
       </c>
       <c r="N861" t="inlineStr">
         <is>
-          <t>{'rate': 4.1854941809063805e-05, 'diff': 19.01, 'diff7d': -5.54, 'ts': 1675055460, 'marketCapUsd': 16837258.025862165, 'availableSupply': 402276464812, 'volume24h': 223656.42316365978, 'volDiff1': 586.4368269122238, 'volDiff7': 52.24060469393129, 'volDiff30': 71.80161871534904, 'bid': 4.698e-05, 'currency': 'USD'}</t>
+          <t>{'rate': 3.9397282122464085e-05, 'diff': -6.26, 'diff7d': 12.35, 'ts': 1675485660, 'marketCapUsd': 15848599.37542586, 'availableSupply': 402276464812, 'volume24h': 59878.746887178924, 'volDiff1': 33.72081270333871, 'volDiff7': 4.346285490879524, 'volDiff30': 105.75469778169571, 'bid': 4.698e-05, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O861" t="n">
-        <v>37015</v>
+        <v>37030</v>
       </c>
       <c r="P861" t="n">
         <v>0</v>
@@ -59341,7 +59403,7 @@
       </c>
       <c r="R861" t="inlineStr">
         <is>
-          <t>37015</t>
+          <t>37030</t>
         </is>
       </c>
       <c r="S861" t="inlineStr"/>
@@ -59584,7 +59646,9 @@
       </c>
       <c r="K865" t="inlineStr"/>
       <c r="L865" t="inlineStr"/>
-      <c r="M865" t="inlineStr"/>
+      <c r="M865" t="n">
+        <v>0</v>
+      </c>
       <c r="N865" t="b">
         <v>0</v>
       </c>
@@ -59842,7 +59906,9 @@
       </c>
       <c r="K869" t="inlineStr"/>
       <c r="L869" t="inlineStr"/>
-      <c r="M869" t="inlineStr"/>
+      <c r="M869" t="n">
+        <v>0</v>
+      </c>
       <c r="N869" t="b">
         <v>0</v>
       </c>
@@ -59908,7 +59974,9 @@
       </c>
       <c r="K870" t="inlineStr"/>
       <c r="L870" t="inlineStr"/>
-      <c r="M870" t="inlineStr"/>
+      <c r="M870" t="n">
+        <v>0</v>
+      </c>
       <c r="N870" t="b">
         <v>0</v>
       </c>
@@ -59974,7 +60042,9 @@
       </c>
       <c r="K871" t="inlineStr"/>
       <c r="L871" t="inlineStr"/>
-      <c r="M871" t="inlineStr"/>
+      <c r="M871" t="n">
+        <v>0</v>
+      </c>
       <c r="N871" t="b">
         <v>0</v>
       </c>
@@ -60552,7 +60622,9 @@
       </c>
       <c r="K880" t="inlineStr"/>
       <c r="L880" t="inlineStr"/>
-      <c r="M880" t="inlineStr"/>
+      <c r="M880" t="n">
+        <v>0</v>
+      </c>
       <c r="N880" t="b">
         <v>0</v>
       </c>
@@ -60678,7 +60750,9 @@
       </c>
       <c r="K882" t="inlineStr"/>
       <c r="L882" t="inlineStr"/>
-      <c r="M882" t="inlineStr"/>
+      <c r="M882" t="n">
+        <v>0</v>
+      </c>
       <c r="N882" t="b">
         <v>0</v>
       </c>
@@ -60804,7 +60878,9 @@
       </c>
       <c r="K884" t="inlineStr"/>
       <c r="L884" t="inlineStr"/>
-      <c r="M884" t="inlineStr"/>
+      <c r="M884" t="n">
+        <v>0</v>
+      </c>
       <c r="N884" t="b">
         <v>0</v>
       </c>
@@ -60856,13 +60932,13 @@
       </c>
       <c r="G885" t="inlineStr"/>
       <c r="H885" t="n">
-        <v>1673694794</v>
+        <v>1675150750</v>
       </c>
       <c r="I885" t="n">
         <v>1</v>
       </c>
       <c r="J885" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K885" t="inlineStr"/>
       <c r="L885" t="inlineStr"/>
@@ -60992,13 +61068,13 @@
         </is>
       </c>
       <c r="H887" t="n">
-        <v>1675055108</v>
+        <v>1675484112</v>
       </c>
       <c r="I887" t="n">
         <v>1</v>
       </c>
       <c r="J887" t="n">
-        <v>4218</v>
+        <v>3914</v>
       </c>
       <c r="K887" t="inlineStr">
         <is>
@@ -61015,7 +61091,7 @@
       </c>
       <c r="N887" t="inlineStr">
         <is>
-          <t>{'rate': 0.028753176956853324, 'diff': 13.71, 'diff7d': 62.36, 'ts': 1675055460, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 100984.7595875041, 'volDiff1': -36.68076488493826, 'volDiff7': 61.100664484140566, 'volDiff30': -92.18366036299228, 'currency': 'USD'}</t>
+          <t>{'rate': 0.004338851880707325, 'diff': 27.71, 'diff7d': -84.35, 'ts': 1675485660, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 56091.41132621, 'volDiff1': -74.54744873706474, 'volDiff7': 30.269642489800475, 'volDiff30': -90.62447100905385, 'diff30d': -55.19551162145547, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O887" t="n">
@@ -61202,13 +61278,13 @@
         </is>
       </c>
       <c r="H890" t="n">
-        <v>1675054413</v>
+        <v>1675482876</v>
       </c>
       <c r="I890" t="n">
         <v>1</v>
       </c>
       <c r="J890" t="n">
-        <v>581</v>
+        <v>631</v>
       </c>
       <c r="K890" t="inlineStr"/>
       <c r="L890" t="inlineStr"/>
@@ -61348,7 +61424,9 @@
       </c>
       <c r="K892" t="inlineStr"/>
       <c r="L892" t="inlineStr"/>
-      <c r="M892" t="inlineStr"/>
+      <c r="M892" t="n">
+        <v>0</v>
+      </c>
       <c r="N892" t="b">
         <v>0</v>
       </c>
@@ -61404,13 +61482,13 @@
         </is>
       </c>
       <c r="H893" t="n">
-        <v>1675037826</v>
+        <v>1675484624</v>
       </c>
       <c r="I893" t="n">
         <v>3</v>
       </c>
       <c r="J893" t="n">
-        <v>44995</v>
+        <v>44984</v>
       </c>
       <c r="K893" t="inlineStr">
         <is>
@@ -61427,7 +61505,7 @@
       </c>
       <c r="N893" t="inlineStr">
         <is>
-          <t>{'rate': 1.6589908669418983e-06, 'diff': -3.87, 'diff7d': -0.56, 'ts': 1675055460, 'marketCapUsd': 422531.1558579716, 'availableSupply': 0, 'volume24h': 85381.23328917, 'volDiff1': -11.370445448922581, 'volDiff7': 19.27165614791717, 'volDiff30': 22.68012535798907, 'diff30d': -54.055777897365545, 'bid': 1.295e-05, 'currency': 'USD'}</t>
+          <t>{'rate': 1.8426268356900563e-06, 'diff': 8.98, 'diff7d': -0.25, 'ts': 1675485660, 'marketCapUsd': 439688.1757108272, 'availableSupply': 0, 'volume24h': 89533.02490016, 'volDiff1': -2.0793273163636883, 'volDiff7': -18.658791640809525, 'volDiff30': 28.50026766327261, 'diff30d': -54.055777897365545, 'bid': 1.295e-05, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O893" t="n">
@@ -61822,13 +61900,13 @@
         </is>
       </c>
       <c r="H899" t="n">
-        <v>1674809480</v>
+        <v>1675236114</v>
       </c>
       <c r="I899" t="n">
         <v>1</v>
       </c>
       <c r="J899" t="n">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K899" t="inlineStr"/>
       <c r="L899" t="inlineStr"/>
@@ -61886,13 +61964,13 @@
       </c>
       <c r="G900" t="inlineStr"/>
       <c r="H900" t="n">
-        <v>1675054602</v>
+        <v>1675484599</v>
       </c>
       <c r="I900" t="n">
         <v>1</v>
       </c>
       <c r="J900" t="n">
-        <v>5462</v>
+        <v>5478</v>
       </c>
       <c r="K900" t="inlineStr">
         <is>
@@ -61909,7 +61987,7 @@
       </c>
       <c r="N900" t="inlineStr">
         <is>
-          <t>{'rate': 0.014368226134824712, 'diff': 1.89, 'diff7d': -10.25, 'ts': 1675055460, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 450957.64532914, 'volDiff1': -4.303273177583108, 'volDiff7': 145.78239603552316, 'currency': 'USD'}</t>
+          <t>{'rate': 0.013927452797096503, 'diff': 0.05, 'diff7d': -3.27, 'ts': 1675485660, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 349313.43952973, 'volDiff1': -13.418888692941437, 'volDiff7': -0.8124860649976569, 'currency': 'USD'}</t>
         </is>
       </c>
       <c r="O900" t="n">
@@ -62096,7 +62174,7 @@
         </is>
       </c>
       <c r="H903" t="n">
-        <v>1675052789</v>
+        <v>1675110899</v>
       </c>
       <c r="I903" t="n">
         <v>61</v>
@@ -62106,7 +62184,9 @@
       </c>
       <c r="K903" t="inlineStr"/>
       <c r="L903" t="inlineStr"/>
-      <c r="M903" t="inlineStr"/>
+      <c r="M903" t="n">
+        <v>0</v>
+      </c>
       <c r="N903" t="b">
         <v>0</v>
       </c>
@@ -62230,17 +62310,19 @@
         </is>
       </c>
       <c r="H905" t="n">
-        <v>1675055606</v>
+        <v>1675485202</v>
       </c>
       <c r="I905" t="n">
         <v>1</v>
       </c>
       <c r="J905" t="n">
-        <v>268</v>
+        <v>396</v>
       </c>
       <c r="K905" t="inlineStr"/>
       <c r="L905" t="inlineStr"/>
-      <c r="M905" t="inlineStr"/>
+      <c r="M905" t="n">
+        <v>0</v>
+      </c>
       <c r="N905" t="b">
         <v>0</v>
       </c>
@@ -62364,13 +62446,13 @@
         </is>
       </c>
       <c r="H907" t="n">
-        <v>1675024872</v>
+        <v>1675464064</v>
       </c>
       <c r="I907" t="n">
         <v>1</v>
       </c>
       <c r="J907" t="n">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="K907" t="inlineStr"/>
       <c r="L907" t="inlineStr"/>
@@ -62632,17 +62714,19 @@
         </is>
       </c>
       <c r="H911" t="n">
-        <v>1675038983</v>
+        <v>1675385789</v>
       </c>
       <c r="I911" t="n">
         <v>1</v>
       </c>
       <c r="J911" t="n">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="K911" t="inlineStr"/>
       <c r="L911" t="inlineStr"/>
-      <c r="M911" t="inlineStr"/>
+      <c r="M911" t="n">
+        <v>0</v>
+      </c>
       <c r="N911" t="b">
         <v>0</v>
       </c>
@@ -62662,6 +62746,412 @@
       </c>
       <c r="S911" t="inlineStr"/>
       <c r="T911" t="inlineStr"/>
+    </row>
+    <row r="912">
+      <c r="A912" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>0xb1133916d67ffabc7a6804ca26fd8a0134109f3e</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>CRIM_PROTOCOL</t>
+        </is>
+      </c>
+      <c r="D912" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="E912" t="inlineStr">
+        <is>
+          <t>CRIM</t>
+        </is>
+      </c>
+      <c r="F912" t="inlineStr">
+        <is>
+          <t>25000000000000000000000000000000</t>
+        </is>
+      </c>
+      <c r="G912" t="inlineStr">
+        <is>
+          <t>0x0d4268fae07462929c415a1ec68e7441b8ad7eed</t>
+        </is>
+      </c>
+      <c r="H912" t="n">
+        <v>1675101539</v>
+      </c>
+      <c r="I912" t="n">
+        <v>1</v>
+      </c>
+      <c r="J912" t="n">
+        <v>18</v>
+      </c>
+      <c r="K912" t="inlineStr"/>
+      <c r="L912" t="inlineStr"/>
+      <c r="M912" t="n">
+        <v>0</v>
+      </c>
+      <c r="N912" t="b">
+        <v>0</v>
+      </c>
+      <c r="O912" t="n">
+        <v>1.25e+31</v>
+      </c>
+      <c r="P912" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q912" t="n">
+        <v>0</v>
+      </c>
+      <c r="R912" t="inlineStr">
+        <is>
+          <t>12500000000000000000000000000000</t>
+        </is>
+      </c>
+      <c r="S912" t="inlineStr"/>
+      <c r="T912" t="inlineStr"/>
+    </row>
+    <row r="913">
+      <c r="A913" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>0x8eb94a06b4716093dbfe335cbdb098deb2dcde1b</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>Half Shiba Inu</t>
+        </is>
+      </c>
+      <c r="D913" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="E913" t="inlineStr">
+        <is>
+          <t>SHIB0.5</t>
+        </is>
+      </c>
+      <c r="F913" t="inlineStr">
+        <is>
+          <t>1000000000000000000000000</t>
+        </is>
+      </c>
+      <c r="G913" t="inlineStr">
+        <is>
+          <t>0x0000000000000000000000000000000000000000</t>
+        </is>
+      </c>
+      <c r="H913" t="n">
+        <v>1675485710</v>
+      </c>
+      <c r="I913" t="n">
+        <v>1</v>
+      </c>
+      <c r="J913" t="n">
+        <v>1219</v>
+      </c>
+      <c r="K913" t="inlineStr"/>
+      <c r="L913" t="inlineStr"/>
+      <c r="M913" t="n">
+        <v>0</v>
+      </c>
+      <c r="N913" t="b">
+        <v>0</v>
+      </c>
+      <c r="O913" t="n">
+        <v>3.27480487e+19</v>
+      </c>
+      <c r="P913" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q913" t="n">
+        <v>0</v>
+      </c>
+      <c r="R913" t="inlineStr">
+        <is>
+          <t>32748048700000000000</t>
+        </is>
+      </c>
+      <c r="S913" t="inlineStr"/>
+      <c r="T913" t="inlineStr"/>
+    </row>
+    <row r="914">
+      <c r="A914" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>0x1e8cc81cdf99c060c3ca646394402b5249b3d3a0</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>VITALIK BOY</t>
+        </is>
+      </c>
+      <c r="D914" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E914" t="inlineStr">
+        <is>
+          <t>VB</t>
+        </is>
+      </c>
+      <c r="F914" t="inlineStr">
+        <is>
+          <t>1000000000000000</t>
+        </is>
+      </c>
+      <c r="G914" t="inlineStr"/>
+      <c r="H914" t="n">
+        <v>1675425364</v>
+      </c>
+      <c r="I914" t="n">
+        <v>1</v>
+      </c>
+      <c r="J914" t="n">
+        <v>114</v>
+      </c>
+      <c r="K914" t="inlineStr"/>
+      <c r="L914" t="inlineStr"/>
+      <c r="M914" t="n">
+        <v>0</v>
+      </c>
+      <c r="N914" t="b">
+        <v>0</v>
+      </c>
+      <c r="O914" t="n">
+        <v>10000000000000</v>
+      </c>
+      <c r="P914" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q914" t="n">
+        <v>0</v>
+      </c>
+      <c r="R914" t="inlineStr">
+        <is>
+          <t>10000000000000</t>
+        </is>
+      </c>
+      <c r="S914" t="inlineStr"/>
+      <c r="T914" t="inlineStr"/>
+    </row>
+    <row r="915">
+      <c r="A915" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>0x675f47cfcbfe976d784c26434ddea025d05064a3</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Image Generation AI Games</t>
+        </is>
+      </c>
+      <c r="D915" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="E915" t="inlineStr">
+        <is>
+          <t>imgnAI</t>
+        </is>
+      </c>
+      <c r="F915" t="inlineStr">
+        <is>
+          <t>1000000000000000000000000000</t>
+        </is>
+      </c>
+      <c r="G915" t="inlineStr"/>
+      <c r="H915" t="n">
+        <v>1675393221</v>
+      </c>
+      <c r="I915" t="n">
+        <v>1</v>
+      </c>
+      <c r="J915" t="n">
+        <v>27</v>
+      </c>
+      <c r="K915" t="inlineStr"/>
+      <c r="L915" t="inlineStr"/>
+      <c r="M915" t="n">
+        <v>0</v>
+      </c>
+      <c r="N915" t="b">
+        <v>0</v>
+      </c>
+      <c r="O915" t="n">
+        <v>2.162596997473202e+26</v>
+      </c>
+      <c r="P915" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q915" t="n">
+        <v>0</v>
+      </c>
+      <c r="R915" t="inlineStr">
+        <is>
+          <t>216259699747320172338772117</t>
+        </is>
+      </c>
+      <c r="S915" t="inlineStr"/>
+      <c r="T915" t="inlineStr"/>
+    </row>
+    <row r="916">
+      <c r="A916" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>0x3819f64f282bf135d62168c1e513280daf905e06</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>Hedron</t>
+        </is>
+      </c>
+      <c r="D916" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E916" t="inlineStr">
+        <is>
+          <t>HDRN</t>
+        </is>
+      </c>
+      <c r="F916" t="inlineStr">
+        <is>
+          <t>115119540513839998364538</t>
+        </is>
+      </c>
+      <c r="G916" t="inlineStr"/>
+      <c r="H916" t="n">
+        <v>1675485224</v>
+      </c>
+      <c r="I916" t="n">
+        <v>889876</v>
+      </c>
+      <c r="J916" t="n">
+        <v>24515</v>
+      </c>
+      <c r="K916" t="inlineStr">
+        <is>
+          <t>https://hedron.pro</t>
+        </is>
+      </c>
+      <c r="L916" t="inlineStr">
+        <is>
+          <t>/images/HDRN3819f64f.png</t>
+        </is>
+      </c>
+      <c r="M916" t="n">
+        <v>0</v>
+      </c>
+      <c r="N916" t="inlineStr">
+        <is>
+          <t>{'rate': 2.2257906811453465e-06, 'diff': 20.16, 'diff7d': 44.47, 'ts': 1675485960, 'marketCapUsd': 0, 'availableSupply': 0, 'volume24h': 1379981.52317852, 'volDiff1': 17.349019345076798, 'volDiff7': 131.74370585665827, 'volDiff30': 13.447721298458532, 'diff30d': 73.69870162071035, 'bid': 1.15e-06, 'currency': 'USD'}</t>
+        </is>
+      </c>
+      <c r="O916" t="n">
+        <v>1</v>
+      </c>
+      <c r="P916" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q916" t="n">
+        <v>0</v>
+      </c>
+      <c r="R916" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="S916" t="inlineStr"/>
+      <c r="T916" t="inlineStr"/>
+    </row>
+    <row r="917">
+      <c r="A917" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>0xdc4d8a6e0c2c43f75875bf2c7e3a1e8423b145e2</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>BlueyardAI</t>
+        </is>
+      </c>
+      <c r="D917" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="E917" t="inlineStr">
+        <is>
+          <t>BYAI</t>
+        </is>
+      </c>
+      <c r="F917" t="inlineStr">
+        <is>
+          <t>20000000000000000000000000000</t>
+        </is>
+      </c>
+      <c r="G917" t="inlineStr">
+        <is>
+          <t>0x52a89ef13cb0331a25e285d48c04fbd668947364</t>
+        </is>
+      </c>
+      <c r="H917" t="n">
+        <v>1675447901</v>
+      </c>
+      <c r="I917" t="n">
+        <v>1</v>
+      </c>
+      <c r="J917" t="n">
+        <v>42</v>
+      </c>
+      <c r="K917" t="inlineStr"/>
+      <c r="L917" t="inlineStr"/>
+      <c r="M917" t="n">
+        <v>0</v>
+      </c>
+      <c r="N917" t="b">
+        <v>0</v>
+      </c>
+      <c r="O917" t="n">
+        <v>1e+28</v>
+      </c>
+      <c r="P917" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q917" t="n">
+        <v>0</v>
+      </c>
+      <c r="R917" t="inlineStr">
+        <is>
+          <t>10000000000000000000000000000</t>
+        </is>
+      </c>
+      <c r="S917" t="inlineStr"/>
+      <c r="T917" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>